<commit_message>
Updated to match ; https://azure.microsoft.com/nl-nl/blog/introducing-the-new-dv3-and-ev3-vm-sizes/
</commit_message>
<xml_diff>
--- a/AzureVMSizes.xlsx
+++ b/AzureVMSizes.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kavaes\Documents\SourceTree\azure-vmchooser-database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karim\Documents\sourcetree\azure-vmchooser-database\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10092"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10095"/>
   </bookViews>
   <sheets>
     <sheet name="AzureVMSizes" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">AzureVMSizes!$A$1:$T$2165</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">AzureVMSizes!$A$1:$T$2169</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="177">
   <si>
     <t>Name</t>
   </si>
@@ -487,6 +487,72 @@
   </si>
   <si>
     <t>6000 - 8000+</t>
+  </si>
+  <si>
+    <t>Standard_D4_v3</t>
+  </si>
+  <si>
+    <t>Standard_D8_v3</t>
+  </si>
+  <si>
+    <t>Standard_D16_v3</t>
+  </si>
+  <si>
+    <t>Standard_D2s_v3</t>
+  </si>
+  <si>
+    <t>Standard_D4s_v3</t>
+  </si>
+  <si>
+    <t>Standard_D8s_v3</t>
+  </si>
+  <si>
+    <t>Standard_D16s_v3</t>
+  </si>
+  <si>
+    <t>Standard_E2s_v3</t>
+  </si>
+  <si>
+    <t>Standard_E4s_v3</t>
+  </si>
+  <si>
+    <t>Standard_E8s_v3</t>
+  </si>
+  <si>
+    <t>Standard_E16s_v3</t>
+  </si>
+  <si>
+    <t>Standard_E32s_v3</t>
+  </si>
+  <si>
+    <t>Standard_E64s_v3</t>
+  </si>
+  <si>
+    <t>Standard_D2_v3</t>
+  </si>
+  <si>
+    <t>Hyperthreaded</t>
+  </si>
+  <si>
+    <t>moderate</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>extremely high</t>
+  </si>
+  <si>
+    <t>Standard_D32_v3</t>
+  </si>
+  <si>
+    <t>Standard_D64_v3</t>
+  </si>
+  <si>
+    <t>Standard_D32s_v3</t>
+  </si>
+  <si>
+    <t>Standard_D64s_v3</t>
   </si>
 </sst>
 </file>
@@ -1008,25 +1074,25 @@
     <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Comma" xfId="42" builtinId="3"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Berekening" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Controlecel" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Gekoppelde cel" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Goed" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Invoer" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Komma" xfId="42" builtinId="3"/>
+    <cellStyle name="Kop 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Kop 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Kop 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Kop 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Neutraal" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Notitie" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Ongeldig" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Titel" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Totaal" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Uitvoer" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Verklarende tekst" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Waarschuwingstekst" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1042,9 +1108,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1082,7 +1148,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1188,7 +1254,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1338,45 +1404,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z117"/>
+  <dimension ref="A1:AA135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2172" ySplit="576" topLeftCell="A94" activePane="bottomRight"/>
-      <selection pane="topRight" activeCell="L1" sqref="L1:L1048576"/>
-      <selection pane="bottomLeft" activeCell="A42" sqref="A42"/>
-      <selection pane="bottomRight" activeCell="L110" sqref="L110:L117"/>
+      <pane xSplit="2670" ySplit="570" topLeftCell="A109" activePane="bottomRight"/>
+      <selection sqref="A1:A1048576"/>
+      <selection pane="topRight" activeCell="AA1" sqref="AA1"/>
+      <selection pane="bottomLeft" activeCell="A129" sqref="A129"/>
+      <selection pane="bottomRight" activeCell="K107" sqref="K107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="21.77734375" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="27.21875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1455,8 +1522,11 @@
       <c r="Z1" s="1" t="s">
         <v>140</v>
       </c>
+      <c r="AA1" s="1" t="s">
+        <v>169</v>
+      </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1544,8 +1614,11 @@
       <c r="Z2" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA2" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1632,8 +1705,11 @@
       <c r="Z3" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA3" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1720,8 +1796,11 @@
       <c r="Z4" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA4" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1808,8 +1887,11 @@
       <c r="Z5" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA5" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1896,8 +1978,11 @@
       <c r="Z6" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA6" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>132</v>
       </c>
@@ -1989,8 +2074,11 @@
       <c r="Z7" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA7" t="s">
+        <v>109</v>
+      </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>133</v>
       </c>
@@ -2082,8 +2170,11 @@
       <c r="Z8" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA8" t="s">
+        <v>109</v>
+      </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>134</v>
       </c>
@@ -2175,8 +2266,11 @@
       <c r="Z9" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA9" t="s">
+        <v>109</v>
+      </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>135</v>
       </c>
@@ -2268,8 +2362,11 @@
       <c r="Z10" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA10" t="s">
+        <v>109</v>
+      </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>136</v>
       </c>
@@ -2361,8 +2458,11 @@
       <c r="Z11" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA11" t="s">
+        <v>109</v>
+      </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>138</v>
       </c>
@@ -2454,8 +2554,11 @@
       <c r="Z12" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA12" t="s">
+        <v>109</v>
+      </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>127</v>
       </c>
@@ -2547,8 +2650,11 @@
       <c r="Z13" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA13" t="s">
+        <v>109</v>
+      </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>131</v>
       </c>
@@ -2640,8 +2746,11 @@
       <c r="Z14" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA14" t="s">
+        <v>109</v>
+      </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>137</v>
       </c>
@@ -2733,8 +2842,11 @@
       <c r="Z15" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA15" t="s">
+        <v>109</v>
+      </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>139</v>
       </c>
@@ -2826,8 +2938,11 @@
       <c r="Z16" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA16" t="s">
+        <v>109</v>
+      </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -2915,8 +3030,11 @@
       <c r="Z17" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA17" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -3003,8 +3121,11 @@
       <c r="Z18" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA18" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>56</v>
       </c>
@@ -3091,8 +3212,11 @@
       <c r="Z19" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA19" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>100</v>
       </c>
@@ -3179,8 +3303,11 @@
       <c r="Z20" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA20" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>101</v>
       </c>
@@ -3267,8 +3394,11 @@
       <c r="Z21" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA21" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -3355,8 +3485,11 @@
       <c r="Z22" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA22" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>58</v>
       </c>
@@ -3443,8 +3576,11 @@
       <c r="Z23" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA23" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -3531,8 +3667,11 @@
       <c r="Z24" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA24" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -3619,8 +3758,11 @@
       <c r="Z25" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA25" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -3707,8 +3849,11 @@
       <c r="Z26" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA26" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>60</v>
       </c>
@@ -3795,8 +3940,11 @@
       <c r="Z27" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA27" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>59</v>
       </c>
@@ -3883,8 +4031,11 @@
       <c r="Z28" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA28" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>23</v>
       </c>
@@ -3971,8 +4122,11 @@
       <c r="Z29" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA29" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -4059,8 +4213,11 @@
       <c r="Z30" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA30" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>25</v>
       </c>
@@ -4147,8 +4304,11 @@
       <c r="Z31" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA31" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>98</v>
       </c>
@@ -4235,8 +4395,11 @@
       <c r="Z32" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA32" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>62</v>
       </c>
@@ -4323,8 +4486,11 @@
       <c r="Z33" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA33" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>61</v>
       </c>
@@ -4411,8 +4577,11 @@
       <c r="Z34" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA34" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>99</v>
       </c>
@@ -4499,8 +4668,11 @@
       <c r="Z35" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA35" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>63</v>
       </c>
@@ -4587,8 +4759,11 @@
       <c r="Z36" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA36" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>26</v>
       </c>
@@ -4675,8 +4850,11 @@
       <c r="Z37" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA37" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>67</v>
       </c>
@@ -4763,8 +4941,11 @@
       <c r="Z38" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA38" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>31</v>
       </c>
@@ -4851,8 +5032,11 @@
       <c r="Z39" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA39" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>68</v>
       </c>
@@ -4939,8 +5123,11 @@
       <c r="Z40" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA40" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>32</v>
       </c>
@@ -5027,8 +5214,11 @@
       <c r="Z41" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA41" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>69</v>
       </c>
@@ -5115,8 +5305,11 @@
       <c r="Z42" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA42" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>33</v>
       </c>
@@ -5203,8 +5396,11 @@
       <c r="Z43" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA43" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>70</v>
       </c>
@@ -5291,8 +5487,11 @@
       <c r="Z44" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA44" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>34</v>
       </c>
@@ -5379,8 +5578,11 @@
       <c r="Z45" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA45" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>35</v>
       </c>
@@ -5467,8 +5669,11 @@
       <c r="Z46" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA46" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>64</v>
       </c>
@@ -5555,8 +5760,11 @@
       <c r="Z47" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA47" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>27</v>
       </c>
@@ -5643,8 +5851,11 @@
       <c r="Z48" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA48" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>65</v>
       </c>
@@ -5731,8 +5942,11 @@
       <c r="Z49" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA49" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>28</v>
       </c>
@@ -5819,8 +6033,11 @@
       <c r="Z50" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA50" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>66</v>
       </c>
@@ -5907,8 +6124,11 @@
       <c r="Z51" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA51" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>29</v>
       </c>
@@ -5995,8 +6215,11 @@
       <c r="Z52" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA52" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>30</v>
       </c>
@@ -6083,8 +6306,11 @@
       <c r="Z53" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA53" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>15</v>
       </c>
@@ -6169,8 +6395,11 @@
       <c r="Z54" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA54" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>41</v>
       </c>
@@ -6255,8 +6484,11 @@
       <c r="Z55" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA55" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>19</v>
       </c>
@@ -6341,8 +6573,11 @@
       <c r="Z56" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA56" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>46</v>
       </c>
@@ -6427,8 +6662,11 @@
       <c r="Z57" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA57" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>20</v>
       </c>
@@ -6513,8 +6751,11 @@
       <c r="Z58" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA58" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>47</v>
       </c>
@@ -6599,8 +6840,11 @@
       <c r="Z59" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA59" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>21</v>
       </c>
@@ -6685,8 +6929,11 @@
       <c r="Z60" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA60" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>48</v>
       </c>
@@ -6771,8 +7018,11 @@
       <c r="Z61" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA61" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>22</v>
       </c>
@@ -6857,8 +7107,11 @@
       <c r="Z62" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA62" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>49</v>
       </c>
@@ -6943,8 +7196,11 @@
       <c r="Z63" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA63" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>50</v>
       </c>
@@ -7029,8 +7285,11 @@
       <c r="Z64" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA64" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>16</v>
       </c>
@@ -7115,8 +7374,11 @@
       <c r="Z65" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA65" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>42</v>
       </c>
@@ -7201,8 +7463,11 @@
       <c r="Z66" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA66" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>17</v>
       </c>
@@ -7287,8 +7552,11 @@
       <c r="Z67" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA67" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>43</v>
       </c>
@@ -7373,8 +7641,11 @@
       <c r="Z68" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA68" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>18</v>
       </c>
@@ -7459,8 +7730,11 @@
       <c r="Z69" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA69" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>44</v>
       </c>
@@ -7545,8 +7819,11 @@
       <c r="Z70" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA70" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>45</v>
       </c>
@@ -7631,8 +7908,11 @@
       <c r="Z71" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA71" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>36</v>
       </c>
@@ -7719,8 +7999,11 @@
       <c r="Z72" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA72" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>40</v>
       </c>
@@ -7807,8 +8090,11 @@
       <c r="Z73" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA73" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>55</v>
       </c>
@@ -7893,8 +8179,11 @@
       <c r="Z74" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA74" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>51</v>
       </c>
@@ -7979,8 +8268,11 @@
       <c r="Z75" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA75" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>37</v>
       </c>
@@ -8067,8 +8359,11 @@
       <c r="Z76" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA76" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>52</v>
       </c>
@@ -8153,8 +8448,11 @@
       <c r="Z77" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA77" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>38</v>
       </c>
@@ -8241,8 +8539,11 @@
       <c r="Z78" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA78" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>53</v>
       </c>
@@ -8327,8 +8628,11 @@
       <c r="Z79" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA79" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>39</v>
       </c>
@@ -8415,8 +8719,11 @@
       <c r="Z80" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA80" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>54</v>
       </c>
@@ -8501,8 +8808,11 @@
       <c r="Z81" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA81" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>74</v>
       </c>
@@ -8589,8 +8899,11 @@
       <c r="Z82" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA82" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>75</v>
       </c>
@@ -8677,8 +8990,11 @@
       <c r="Z83" s="1" t="s">
         <v>144</v>
       </c>
+      <c r="AA83" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>76</v>
       </c>
@@ -8765,8 +9081,11 @@
       <c r="Z84" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA84" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>77</v>
       </c>
@@ -8853,8 +9172,11 @@
       <c r="Z85" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA85" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>78</v>
       </c>
@@ -8941,8 +9263,11 @@
       <c r="Z86" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA86" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>79</v>
       </c>
@@ -9027,8 +9352,11 @@
       <c r="Z87" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA87" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>80</v>
       </c>
@@ -9113,8 +9441,11 @@
       <c r="Z88" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA88" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>81</v>
       </c>
@@ -9199,8 +9530,11 @@
       <c r="Z89" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA89" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>82</v>
       </c>
@@ -9285,8 +9619,11 @@
       <c r="Z90" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA90" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>83</v>
       </c>
@@ -9371,8 +9708,11 @@
       <c r="Z91" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA91" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>89</v>
       </c>
@@ -9459,8 +9799,11 @@
       <c r="Z92" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA92" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>91</v>
       </c>
@@ -9547,8 +9890,11 @@
       <c r="Z93" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA93" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>93</v>
       </c>
@@ -9635,8 +9981,11 @@
       <c r="Z94" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA94" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>92</v>
       </c>
@@ -9723,8 +10072,11 @@
       <c r="Z95" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA95" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>88</v>
       </c>
@@ -9811,8 +10163,11 @@
       <c r="Z96" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA96" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>90</v>
       </c>
@@ -9899,8 +10254,11 @@
       <c r="Z97" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA97" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>86</v>
       </c>
@@ -9985,8 +10343,11 @@
       <c r="Z98" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA98" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>87</v>
       </c>
@@ -10071,8 +10432,11 @@
       <c r="Z99" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA99" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="100" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>84</v>
       </c>
@@ -10157,8 +10521,11 @@
       <c r="Z100" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA100" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="101" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>85</v>
       </c>
@@ -10243,8 +10610,11 @@
       <c r="Z101" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA101" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="102" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>126</v>
       </c>
@@ -10334,8 +10704,11 @@
       <c r="Z102" s="1" t="s">
         <v>109</v>
       </c>
+      <c r="AA102" t="s">
+        <v>109</v>
+      </c>
     </row>
-    <row r="103" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>103</v>
       </c>
@@ -10425,8 +10798,11 @@
       <c r="Z103" s="1" t="s">
         <v>109</v>
       </c>
+      <c r="AA103" t="s">
+        <v>109</v>
+      </c>
     </row>
-    <row r="104" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>102</v>
       </c>
@@ -10516,8 +10892,11 @@
       <c r="Z104" s="1" t="s">
         <v>109</v>
       </c>
+      <c r="AA104" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="105" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>95</v>
       </c>
@@ -10609,8 +10988,11 @@
       <c r="Z105" s="1" t="s">
         <v>109</v>
       </c>
+      <c r="AA105" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="106" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>96</v>
       </c>
@@ -10702,8 +11084,11 @@
       <c r="Z106" s="1" t="s">
         <v>109</v>
       </c>
+      <c r="AA106" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="107" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>97</v>
       </c>
@@ -10795,8 +11180,11 @@
       <c r="Z107" s="1" t="s">
         <v>109</v>
       </c>
+      <c r="AA107" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="108" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>94</v>
       </c>
@@ -10888,8 +11276,11 @@
       <c r="Z108" s="1" t="s">
         <v>109</v>
       </c>
+      <c r="AA108" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="109" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>72</v>
       </c>
@@ -10981,8 +11372,11 @@
       <c r="Z109" s="1" t="s">
         <v>109</v>
       </c>
+      <c r="AA109" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="110" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>73</v>
       </c>
@@ -11074,8 +11468,11 @@
       <c r="Z110" s="1" t="s">
         <v>109</v>
       </c>
+      <c r="AA110" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="111" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>71</v>
       </c>
@@ -11167,8 +11564,11 @@
       <c r="Z111" s="1" t="s">
         <v>109</v>
       </c>
+      <c r="AA111" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="112" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>145</v>
       </c>
@@ -11202,11 +11602,11 @@
         <f>16*1024</f>
         <v>16384</v>
       </c>
-      <c r="K112" s="1" t="s">
-        <v>120</v>
+      <c r="K112" s="1">
+        <v>2</v>
       </c>
       <c r="L112" s="1" t="s">
-        <v>120</v>
+        <v>170</v>
       </c>
       <c r="M112" s="1">
         <v>4</v>
@@ -11223,11 +11623,11 @@
         <f>M112*60</f>
         <v>240</v>
       </c>
-      <c r="Q112" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="R112" s="1" t="s">
-        <v>120</v>
+      <c r="Q112" s="1">
+        <v>3000</v>
+      </c>
+      <c r="R112" s="1">
+        <v>46</v>
       </c>
       <c r="S112" s="1" t="s">
         <v>120</v>
@@ -11253,8 +11653,11 @@
       <c r="Z112" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA112" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="113" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>146</v>
       </c>
@@ -11288,32 +11691,32 @@
         <f>32*1024</f>
         <v>32768</v>
       </c>
-      <c r="K113" s="1" t="s">
-        <v>120</v>
+      <c r="K113" s="1">
+        <v>2</v>
       </c>
       <c r="L113" s="1" t="s">
-        <v>120</v>
+        <v>170</v>
       </c>
       <c r="M113" s="1">
         <v>8</v>
       </c>
       <c r="N113" s="1">
-        <f t="shared" ref="N113:N117" si="45">M113*4*1024</f>
+        <f t="shared" ref="N113:N127" si="45">M113*4*1024</f>
         <v>32768</v>
       </c>
       <c r="O113" s="1">
-        <f t="shared" ref="O113:O117" si="46">M113*500</f>
+        <f t="shared" ref="O113:O127" si="46">M113*500</f>
         <v>4000</v>
       </c>
       <c r="P113" s="1">
-        <f t="shared" ref="P113:P117" si="47">M113*60</f>
+        <f t="shared" ref="P113:P127" si="47">M113*60</f>
         <v>480</v>
       </c>
-      <c r="Q113" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="R113" s="1" t="s">
-        <v>120</v>
+      <c r="Q113" s="1">
+        <v>6000</v>
+      </c>
+      <c r="R113" s="1">
+        <v>93</v>
       </c>
       <c r="S113" s="1" t="s">
         <v>120</v>
@@ -11339,8 +11742,11 @@
       <c r="Z113" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA113" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="114" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>147</v>
       </c>
@@ -11374,11 +11780,11 @@
         <f>64*1024</f>
         <v>65536</v>
       </c>
-      <c r="K114" s="1" t="s">
-        <v>120</v>
+      <c r="K114" s="1">
+        <v>4</v>
       </c>
       <c r="L114" s="1" t="s">
-        <v>120</v>
+        <v>171</v>
       </c>
       <c r="M114" s="1">
         <v>16</v>
@@ -11395,11 +11801,11 @@
         <f t="shared" si="47"/>
         <v>960</v>
       </c>
-      <c r="Q114" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="R114" s="1" t="s">
-        <v>120</v>
+      <c r="Q114" s="1">
+        <v>12000</v>
+      </c>
+      <c r="R114" s="1">
+        <v>187</v>
       </c>
       <c r="S114" s="1" t="s">
         <v>120</v>
@@ -11425,8 +11831,11 @@
       <c r="Z114" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA114" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="115" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>148</v>
       </c>
@@ -11460,11 +11869,11 @@
         <f>128*1024</f>
         <v>131072</v>
       </c>
-      <c r="K115" s="1" t="s">
-        <v>120</v>
+      <c r="K115" s="1">
+        <v>4</v>
       </c>
       <c r="L115" s="1" t="s">
-        <v>120</v>
+        <v>171</v>
       </c>
       <c r="M115" s="1">
         <v>32</v>
@@ -11481,11 +11890,11 @@
         <f t="shared" si="47"/>
         <v>1920</v>
       </c>
-      <c r="Q115" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="R115" s="1" t="s">
-        <v>120</v>
+      <c r="Q115" s="1">
+        <v>24000</v>
+      </c>
+      <c r="R115" s="1">
+        <v>375</v>
       </c>
       <c r="S115" s="1" t="s">
         <v>120</v>
@@ -11511,8 +11920,11 @@
       <c r="Z115" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA115" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="116" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>149</v>
       </c>
@@ -11546,11 +11958,11 @@
         <f>256*1024</f>
         <v>262144</v>
       </c>
-      <c r="K116" s="1" t="s">
-        <v>120</v>
+      <c r="K116" s="1">
+        <v>8</v>
       </c>
       <c r="L116" s="1" t="s">
-        <v>120</v>
+        <v>172</v>
       </c>
       <c r="M116" s="1">
         <v>64</v>
@@ -11567,11 +11979,11 @@
         <f t="shared" si="47"/>
         <v>3840</v>
       </c>
-      <c r="Q116" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="R116" s="1" t="s">
-        <v>120</v>
+      <c r="Q116" s="1">
+        <v>48000</v>
+      </c>
+      <c r="R116" s="1">
+        <v>750</v>
       </c>
       <c r="S116" s="1" t="s">
         <v>120</v>
@@ -11597,8 +12009,11 @@
       <c r="Z116" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA116" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="117" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>150</v>
       </c>
@@ -11632,11 +12047,11 @@
         <f>432*1024</f>
         <v>442368</v>
       </c>
-      <c r="K117" s="1" t="s">
-        <v>120</v>
+      <c r="K117" s="1">
+        <v>8</v>
       </c>
       <c r="L117" s="1" t="s">
-        <v>120</v>
+        <v>172</v>
       </c>
       <c r="M117" s="1">
         <v>64</v>
@@ -11653,11 +12068,11 @@
         <f t="shared" si="47"/>
         <v>3840</v>
       </c>
-      <c r="Q117" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="R117" s="1" t="s">
-        <v>120</v>
+      <c r="Q117" s="1">
+        <v>96000</v>
+      </c>
+      <c r="R117" s="1">
+        <v>1000</v>
       </c>
       <c r="S117" s="1" t="s">
         <v>120</v>
@@ -11683,11 +12098,1608 @@
       <c r="Z117" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AA117" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="118" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>168</v>
+      </c>
+      <c r="B118" t="s">
+        <v>129</v>
+      </c>
+      <c r="C118" s="1">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F118" s="1" t="str">
+        <f t="shared" ref="F118:F127" si="48">IFERROR(E118*I118,"Unknown")</f>
+        <v>Unknown</v>
+      </c>
+      <c r="G118" s="2" t="str">
+        <f t="shared" ref="G118:G127" si="49">IFERROR(C118/F118*1000,"Unknown")</f>
+        <v>Unknown</v>
+      </c>
+      <c r="H118" t="s">
+        <v>108</v>
+      </c>
+      <c r="I118">
+        <v>2</v>
+      </c>
+      <c r="J118">
+        <f>8*1024</f>
+        <v>8192</v>
+      </c>
+      <c r="K118">
+        <v>2</v>
+      </c>
+      <c r="L118" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="M118" s="1">
+        <v>4</v>
+      </c>
+      <c r="N118" s="1">
+        <f t="shared" si="45"/>
+        <v>16384</v>
+      </c>
+      <c r="O118" s="1">
+        <f t="shared" si="46"/>
+        <v>2000</v>
+      </c>
+      <c r="P118" s="1">
+        <f t="shared" si="47"/>
+        <v>240</v>
+      </c>
+      <c r="Q118">
+        <f>O118</f>
+        <v>2000</v>
+      </c>
+      <c r="R118">
+        <v>3000</v>
+      </c>
+      <c r="S118" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="T118">
+        <v>50</v>
+      </c>
+      <c r="U118" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="V118" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="W118" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="X118" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y118" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z118" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA118" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="119" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>155</v>
+      </c>
+      <c r="B119" t="s">
+        <v>129</v>
+      </c>
+      <c r="C119" s="1">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F119" s="1" t="str">
+        <f t="shared" si="48"/>
+        <v>Unknown</v>
+      </c>
+      <c r="G119" s="2" t="str">
+        <f t="shared" si="49"/>
+        <v>Unknown</v>
+      </c>
+      <c r="H119" t="s">
+        <v>108</v>
+      </c>
+      <c r="I119">
+        <v>4</v>
+      </c>
+      <c r="J119">
+        <f>16*1024</f>
+        <v>16384</v>
+      </c>
+      <c r="K119">
+        <v>2</v>
+      </c>
+      <c r="L119" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="M119" s="1">
+        <v>8</v>
+      </c>
+      <c r="N119" s="1">
+        <f t="shared" si="45"/>
+        <v>32768</v>
+      </c>
+      <c r="O119" s="1">
+        <f t="shared" si="46"/>
+        <v>4000</v>
+      </c>
+      <c r="P119" s="1">
+        <f t="shared" si="47"/>
+        <v>480</v>
+      </c>
+      <c r="Q119">
+        <f>O119</f>
+        <v>4000</v>
+      </c>
+      <c r="R119">
+        <v>6000</v>
+      </c>
+      <c r="S119" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="T119">
+        <v>100</v>
+      </c>
+      <c r="U119" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="V119" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="W119" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="X119" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y119" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z119" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA119" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="120" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>156</v>
+      </c>
+      <c r="B120" t="s">
+        <v>129</v>
+      </c>
+      <c r="C120" s="1">
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F120" s="1" t="str">
+        <f t="shared" si="48"/>
+        <v>Unknown</v>
+      </c>
+      <c r="G120" s="2" t="str">
+        <f t="shared" si="49"/>
+        <v>Unknown</v>
+      </c>
+      <c r="H120" t="s">
+        <v>108</v>
+      </c>
+      <c r="I120">
+        <v>8</v>
+      </c>
+      <c r="J120">
+        <f>32*1024</f>
+        <v>32768</v>
+      </c>
+      <c r="K120">
+        <v>4</v>
+      </c>
+      <c r="L120" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="M120" s="1">
+        <v>16</v>
+      </c>
+      <c r="N120" s="1">
+        <f t="shared" si="45"/>
+        <v>65536</v>
+      </c>
+      <c r="O120" s="1">
+        <f t="shared" si="46"/>
+        <v>8000</v>
+      </c>
+      <c r="P120" s="1">
+        <f t="shared" si="47"/>
+        <v>960</v>
+      </c>
+      <c r="Q120">
+        <f>O120</f>
+        <v>8000</v>
+      </c>
+      <c r="R120">
+        <v>12000</v>
+      </c>
+      <c r="S120" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="T120">
+        <v>200</v>
+      </c>
+      <c r="U120" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="V120" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="W120" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="X120" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y120" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z120" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA120" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="121" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>157</v>
+      </c>
+      <c r="B121" t="s">
+        <v>129</v>
+      </c>
+      <c r="C121" s="1">
+        <v>0.81</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F121" s="1" t="str">
+        <f t="shared" si="48"/>
+        <v>Unknown</v>
+      </c>
+      <c r="G121" s="2" t="str">
+        <f t="shared" si="49"/>
+        <v>Unknown</v>
+      </c>
+      <c r="H121" t="s">
+        <v>108</v>
+      </c>
+      <c r="I121">
+        <v>16</v>
+      </c>
+      <c r="J121">
+        <f>64*1024</f>
+        <v>65536</v>
+      </c>
+      <c r="K121">
+        <v>8</v>
+      </c>
+      <c r="L121" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="M121" s="1">
+        <v>32</v>
+      </c>
+      <c r="N121" s="1">
+        <f t="shared" si="45"/>
+        <v>131072</v>
+      </c>
+      <c r="O121" s="1">
+        <f t="shared" si="46"/>
+        <v>16000</v>
+      </c>
+      <c r="P121" s="1">
+        <f t="shared" si="47"/>
+        <v>1920</v>
+      </c>
+      <c r="Q121">
+        <f>O121</f>
+        <v>16000</v>
+      </c>
+      <c r="R121">
+        <v>24000</v>
+      </c>
+      <c r="S121" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="T121">
+        <v>400</v>
+      </c>
+      <c r="U121" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="V121" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="W121" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="X121" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y121" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z121" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA121" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="122" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>173</v>
+      </c>
+      <c r="B122" t="s">
+        <v>129</v>
+      </c>
+      <c r="C122" s="1">
+        <v>1.62</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F122" s="1" t="str">
+        <f t="shared" ref="F122:F123" si="50">IFERROR(E122*I122,"Unknown")</f>
+        <v>Unknown</v>
+      </c>
+      <c r="G122" s="2" t="str">
+        <f t="shared" ref="G122:G123" si="51">IFERROR(C122/F122*1000,"Unknown")</f>
+        <v>Unknown</v>
+      </c>
+      <c r="H122" t="s">
+        <v>108</v>
+      </c>
+      <c r="I122">
+        <v>32</v>
+      </c>
+      <c r="J122">
+        <f>128*1024</f>
+        <v>131072</v>
+      </c>
+      <c r="K122" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L122" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="M122" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="N122" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="O122" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="P122" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q122" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="R122" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="S122" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="T122" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="U122" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="V122" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="W122" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="X122" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y122" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z122" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA122" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="123" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>174</v>
+      </c>
+      <c r="B123" t="s">
+        <v>129</v>
+      </c>
+      <c r="C123" s="1">
+        <v>3.2389999999999999</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F123" s="1" t="str">
+        <f t="shared" si="50"/>
+        <v>Unknown</v>
+      </c>
+      <c r="G123" s="2" t="str">
+        <f t="shared" si="51"/>
+        <v>Unknown</v>
+      </c>
+      <c r="H123" t="s">
+        <v>108</v>
+      </c>
+      <c r="I123">
+        <v>64</v>
+      </c>
+      <c r="J123">
+        <f>256*1024</f>
+        <v>262144</v>
+      </c>
+      <c r="K123" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L123" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="M123" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="N123" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="O123" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="P123" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q123" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="R123" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="S123" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="T123" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="U123" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="V123" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="W123" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="X123" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y123" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z123" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA123" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="124" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>158</v>
+      </c>
+      <c r="B124" t="s">
+        <v>129</v>
+      </c>
+      <c r="C124" s="1">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F124" s="1" t="str">
+        <f t="shared" si="48"/>
+        <v>Unknown</v>
+      </c>
+      <c r="G124" s="2" t="str">
+        <f t="shared" si="49"/>
+        <v>Unknown</v>
+      </c>
+      <c r="H124" t="s">
+        <v>109</v>
+      </c>
+      <c r="I124">
+        <v>2</v>
+      </c>
+      <c r="J124">
+        <f>8*1024</f>
+        <v>8192</v>
+      </c>
+      <c r="K124">
+        <v>2</v>
+      </c>
+      <c r="L124" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="M124" s="1">
+        <v>4</v>
+      </c>
+      <c r="N124" s="1">
+        <f t="shared" si="45"/>
+        <v>16384</v>
+      </c>
+      <c r="O124" s="1">
+        <f t="shared" si="46"/>
+        <v>2000</v>
+      </c>
+      <c r="P124" s="1">
+        <f t="shared" si="47"/>
+        <v>240</v>
+      </c>
+      <c r="Q124">
+        <v>4000</v>
+      </c>
+      <c r="R124">
+        <v>32</v>
+      </c>
+      <c r="S124" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="T124">
+        <v>50</v>
+      </c>
+      <c r="U124" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="V124" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="W124" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="X124" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y124" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z124" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA124" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="125" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>159</v>
+      </c>
+      <c r="B125" t="s">
+        <v>129</v>
+      </c>
+      <c r="C125" s="1">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F125" s="1" t="str">
+        <f t="shared" si="48"/>
+        <v>Unknown</v>
+      </c>
+      <c r="G125" s="2" t="str">
+        <f t="shared" si="49"/>
+        <v>Unknown</v>
+      </c>
+      <c r="H125" t="s">
+        <v>109</v>
+      </c>
+      <c r="I125">
+        <v>4</v>
+      </c>
+      <c r="J125">
+        <f>16*1024</f>
+        <v>16384</v>
+      </c>
+      <c r="K125">
+        <v>2</v>
+      </c>
+      <c r="L125" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="M125" s="1">
+        <v>8</v>
+      </c>
+      <c r="N125" s="1">
+        <f t="shared" si="45"/>
+        <v>32768</v>
+      </c>
+      <c r="O125" s="1">
+        <f t="shared" si="46"/>
+        <v>4000</v>
+      </c>
+      <c r="P125" s="1">
+        <f t="shared" si="47"/>
+        <v>480</v>
+      </c>
+      <c r="Q125">
+        <v>8000</v>
+      </c>
+      <c r="R125">
+        <v>64</v>
+      </c>
+      <c r="S125" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="T125">
+        <v>100</v>
+      </c>
+      <c r="U125" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="V125" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="W125" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="X125" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y125" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z125" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA125" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="126" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>160</v>
+      </c>
+      <c r="B126" t="s">
+        <v>129</v>
+      </c>
+      <c r="C126" s="1">
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F126" s="1" t="str">
+        <f t="shared" si="48"/>
+        <v>Unknown</v>
+      </c>
+      <c r="G126" s="2" t="str">
+        <f t="shared" si="49"/>
+        <v>Unknown</v>
+      </c>
+      <c r="H126" t="s">
+        <v>109</v>
+      </c>
+      <c r="I126">
+        <v>8</v>
+      </c>
+      <c r="J126">
+        <f>32*1024</f>
+        <v>32768</v>
+      </c>
+      <c r="K126">
+        <v>4</v>
+      </c>
+      <c r="L126" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="M126" s="1">
+        <v>16</v>
+      </c>
+      <c r="N126" s="1">
+        <f t="shared" si="45"/>
+        <v>65536</v>
+      </c>
+      <c r="O126" s="1">
+        <f t="shared" si="46"/>
+        <v>8000</v>
+      </c>
+      <c r="P126" s="1">
+        <f t="shared" si="47"/>
+        <v>960</v>
+      </c>
+      <c r="Q126">
+        <v>16000</v>
+      </c>
+      <c r="R126">
+        <v>128</v>
+      </c>
+      <c r="S126" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="T126">
+        <v>200</v>
+      </c>
+      <c r="U126" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="V126" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="W126" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="X126" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y126" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z126" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA126" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="127" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>161</v>
+      </c>
+      <c r="B127" t="s">
+        <v>129</v>
+      </c>
+      <c r="C127" s="1">
+        <v>0.81</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F127" s="1" t="str">
+        <f t="shared" si="48"/>
+        <v>Unknown</v>
+      </c>
+      <c r="G127" s="2" t="str">
+        <f t="shared" si="49"/>
+        <v>Unknown</v>
+      </c>
+      <c r="H127" t="s">
+        <v>109</v>
+      </c>
+      <c r="I127">
+        <v>16</v>
+      </c>
+      <c r="J127">
+        <f>64*1024</f>
+        <v>65536</v>
+      </c>
+      <c r="K127">
+        <v>8</v>
+      </c>
+      <c r="L127" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="M127" s="1">
+        <v>32</v>
+      </c>
+      <c r="N127" s="1">
+        <f t="shared" si="45"/>
+        <v>131072</v>
+      </c>
+      <c r="O127" s="1">
+        <f t="shared" si="46"/>
+        <v>16000</v>
+      </c>
+      <c r="P127" s="1">
+        <f t="shared" si="47"/>
+        <v>1920</v>
+      </c>
+      <c r="Q127">
+        <v>32000</v>
+      </c>
+      <c r="R127">
+        <v>256</v>
+      </c>
+      <c r="S127" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="T127">
+        <v>400</v>
+      </c>
+      <c r="U127" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="V127" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="W127" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="X127" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y127" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z127" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA127" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="128" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>175</v>
+      </c>
+      <c r="B128" t="s">
+        <v>129</v>
+      </c>
+      <c r="C128" s="1">
+        <v>1.62</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F128" s="1" t="str">
+        <f t="shared" ref="F128:F129" si="52">IFERROR(E128*I128,"Unknown")</f>
+        <v>Unknown</v>
+      </c>
+      <c r="G128" s="2" t="str">
+        <f t="shared" ref="G128:G129" si="53">IFERROR(C128/F128*1000,"Unknown")</f>
+        <v>Unknown</v>
+      </c>
+      <c r="H128" t="s">
+        <v>109</v>
+      </c>
+      <c r="I128">
+        <v>32</v>
+      </c>
+      <c r="J128">
+        <f>128*1024</f>
+        <v>131072</v>
+      </c>
+      <c r="K128" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L128" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="M128" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="N128" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="O128" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="P128" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q128" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="R128" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="S128" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="T128" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="U128" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="V128" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="W128" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="X128" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y128" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z128" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA128" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="129" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>176</v>
+      </c>
+      <c r="B129" t="s">
+        <v>129</v>
+      </c>
+      <c r="C129" s="1">
+        <v>3.2389999999999999</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F129" s="1" t="str">
+        <f t="shared" si="52"/>
+        <v>Unknown</v>
+      </c>
+      <c r="G129" s="2" t="str">
+        <f t="shared" si="53"/>
+        <v>Unknown</v>
+      </c>
+      <c r="H129" t="s">
+        <v>109</v>
+      </c>
+      <c r="I129">
+        <v>64</v>
+      </c>
+      <c r="J129">
+        <f>256*1024</f>
+        <v>262144</v>
+      </c>
+      <c r="K129" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L129" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="M129" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="N129" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="O129" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="P129" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q129" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="R129" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="S129" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="T129" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="U129" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="V129" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="W129" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="X129" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y129" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z129" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA129" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="130" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>162</v>
+      </c>
+      <c r="B130" t="s">
+        <v>129</v>
+      </c>
+      <c r="C130" s="1">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F130" s="1" t="str">
+        <f t="shared" ref="F130:F135" si="54">IFERROR(E130*I130,"Unknown")</f>
+        <v>Unknown</v>
+      </c>
+      <c r="G130" s="2" t="str">
+        <f t="shared" ref="G130:G135" si="55">IFERROR(C130/F130*1000,"Unknown")</f>
+        <v>Unknown</v>
+      </c>
+      <c r="H130" t="s">
+        <v>109</v>
+      </c>
+      <c r="I130">
+        <v>2</v>
+      </c>
+      <c r="J130">
+        <f>16*1024</f>
+        <v>16384</v>
+      </c>
+      <c r="K130" s="1">
+        <v>2</v>
+      </c>
+      <c r="L130" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="M130" s="1">
+        <v>4</v>
+      </c>
+      <c r="N130" s="1">
+        <f>M130*4*1024</f>
+        <v>16384</v>
+      </c>
+      <c r="O130" s="1">
+        <f>M130*500</f>
+        <v>2000</v>
+      </c>
+      <c r="P130" s="1">
+        <f>M130*60</f>
+        <v>240</v>
+      </c>
+      <c r="Q130" s="1">
+        <v>4000</v>
+      </c>
+      <c r="R130" s="1">
+        <v>32</v>
+      </c>
+      <c r="S130" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="T130" s="1">
+        <v>32</v>
+      </c>
+      <c r="U130" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="V130" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="W130" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="X130" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y130" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z130" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA130" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="131" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>163</v>
+      </c>
+      <c r="B131" t="s">
+        <v>129</v>
+      </c>
+      <c r="C131" s="1">
+        <v>0.27</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F131" s="1" t="str">
+        <f t="shared" si="54"/>
+        <v>Unknown</v>
+      </c>
+      <c r="G131" s="2" t="str">
+        <f t="shared" si="55"/>
+        <v>Unknown</v>
+      </c>
+      <c r="H131" t="s">
+        <v>109</v>
+      </c>
+      <c r="I131">
+        <v>4</v>
+      </c>
+      <c r="J131">
+        <f>32*1024</f>
+        <v>32768</v>
+      </c>
+      <c r="K131" s="1">
+        <v>2</v>
+      </c>
+      <c r="L131" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="M131" s="1">
+        <v>8</v>
+      </c>
+      <c r="N131" s="1">
+        <f t="shared" ref="N131:N135" si="56">M131*4*1024</f>
+        <v>32768</v>
+      </c>
+      <c r="O131" s="1">
+        <f t="shared" ref="O131:O135" si="57">M131*500</f>
+        <v>4000</v>
+      </c>
+      <c r="P131" s="1">
+        <f t="shared" ref="P131:P135" si="58">M131*60</f>
+        <v>480</v>
+      </c>
+      <c r="Q131" s="1">
+        <v>8000</v>
+      </c>
+      <c r="R131" s="1">
+        <v>64</v>
+      </c>
+      <c r="S131" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="T131" s="1">
+        <v>64</v>
+      </c>
+      <c r="U131" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="V131" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="W131" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="X131" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y131" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z131" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA131" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="132" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>164</v>
+      </c>
+      <c r="B132" t="s">
+        <v>129</v>
+      </c>
+      <c r="C132" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F132" s="1" t="str">
+        <f t="shared" si="54"/>
+        <v>Unknown</v>
+      </c>
+      <c r="G132" s="2" t="str">
+        <f t="shared" si="55"/>
+        <v>Unknown</v>
+      </c>
+      <c r="H132" t="s">
+        <v>109</v>
+      </c>
+      <c r="I132">
+        <v>8</v>
+      </c>
+      <c r="J132">
+        <f>64*1024</f>
+        <v>65536</v>
+      </c>
+      <c r="K132" s="1">
+        <v>4</v>
+      </c>
+      <c r="L132" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="M132" s="1">
+        <v>16</v>
+      </c>
+      <c r="N132" s="1">
+        <f t="shared" si="56"/>
+        <v>65536</v>
+      </c>
+      <c r="O132" s="1">
+        <f t="shared" si="57"/>
+        <v>8000</v>
+      </c>
+      <c r="P132" s="1">
+        <f t="shared" si="58"/>
+        <v>960</v>
+      </c>
+      <c r="Q132" s="1">
+        <v>16000</v>
+      </c>
+      <c r="R132" s="1">
+        <v>128</v>
+      </c>
+      <c r="S132" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="T132" s="1">
+        <v>128</v>
+      </c>
+      <c r="U132" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="V132" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="W132" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="X132" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y132" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z132" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA132" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="133" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>165</v>
+      </c>
+      <c r="B133" t="s">
+        <v>129</v>
+      </c>
+      <c r="C133" s="1">
+        <v>1.08</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F133" s="1" t="str">
+        <f t="shared" si="54"/>
+        <v>Unknown</v>
+      </c>
+      <c r="G133" s="2" t="str">
+        <f t="shared" si="55"/>
+        <v>Unknown</v>
+      </c>
+      <c r="H133" t="s">
+        <v>109</v>
+      </c>
+      <c r="I133">
+        <v>16</v>
+      </c>
+      <c r="J133">
+        <f>128*1024</f>
+        <v>131072</v>
+      </c>
+      <c r="K133" s="1">
+        <v>4</v>
+      </c>
+      <c r="L133" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="M133" s="1">
+        <v>32</v>
+      </c>
+      <c r="N133" s="1">
+        <f t="shared" si="56"/>
+        <v>131072</v>
+      </c>
+      <c r="O133" s="1">
+        <f t="shared" si="57"/>
+        <v>16000</v>
+      </c>
+      <c r="P133" s="1">
+        <f t="shared" si="58"/>
+        <v>1920</v>
+      </c>
+      <c r="Q133" s="1">
+        <v>32000</v>
+      </c>
+      <c r="R133" s="1">
+        <v>256</v>
+      </c>
+      <c r="S133" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="T133" s="1">
+        <v>256</v>
+      </c>
+      <c r="U133" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="V133" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="W133" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="X133" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y133" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z133" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA133" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="134" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>166</v>
+      </c>
+      <c r="B134" t="s">
+        <v>129</v>
+      </c>
+      <c r="C134" s="1">
+        <v>2.1589999999999998</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F134" s="1" t="str">
+        <f t="shared" si="54"/>
+        <v>Unknown</v>
+      </c>
+      <c r="G134" s="2" t="str">
+        <f t="shared" si="55"/>
+        <v>Unknown</v>
+      </c>
+      <c r="H134" t="s">
+        <v>109</v>
+      </c>
+      <c r="I134">
+        <v>32</v>
+      </c>
+      <c r="J134">
+        <f>256*1024</f>
+        <v>262144</v>
+      </c>
+      <c r="K134" s="1">
+        <v>8</v>
+      </c>
+      <c r="L134" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="M134" s="1">
+        <v>64</v>
+      </c>
+      <c r="N134" s="1">
+        <f t="shared" si="56"/>
+        <v>262144</v>
+      </c>
+      <c r="O134" s="1">
+        <f t="shared" si="57"/>
+        <v>32000</v>
+      </c>
+      <c r="P134" s="1">
+        <f t="shared" si="58"/>
+        <v>3840</v>
+      </c>
+      <c r="Q134" s="1">
+        <v>64000</v>
+      </c>
+      <c r="R134" s="1">
+        <v>512</v>
+      </c>
+      <c r="S134" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="T134" s="1">
+        <v>512</v>
+      </c>
+      <c r="U134" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="V134" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="W134" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="X134" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y134" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z134" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA134" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="135" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>167</v>
+      </c>
+      <c r="B135" t="s">
+        <v>129</v>
+      </c>
+      <c r="C135" s="1">
+        <v>4.07</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F135" s="1" t="str">
+        <f t="shared" si="54"/>
+        <v>Unknown</v>
+      </c>
+      <c r="G135" s="2" t="str">
+        <f t="shared" si="55"/>
+        <v>Unknown</v>
+      </c>
+      <c r="H135" t="s">
+        <v>109</v>
+      </c>
+      <c r="I135">
+        <v>64</v>
+      </c>
+      <c r="J135">
+        <f>432*1024</f>
+        <v>442368</v>
+      </c>
+      <c r="K135" s="1">
+        <v>8</v>
+      </c>
+      <c r="L135" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="M135" s="1">
+        <v>64</v>
+      </c>
+      <c r="N135" s="1">
+        <f t="shared" si="56"/>
+        <v>262144</v>
+      </c>
+      <c r="O135" s="1">
+        <f t="shared" si="57"/>
+        <v>32000</v>
+      </c>
+      <c r="P135" s="1">
+        <f t="shared" si="58"/>
+        <v>3840</v>
+      </c>
+      <c r="Q135" s="1">
+        <v>128000</v>
+      </c>
+      <c r="R135" s="1">
+        <v>1024</v>
+      </c>
+      <c r="S135" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="T135" s="1">
+        <v>868</v>
+      </c>
+      <c r="U135" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="V135" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="W135" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="X135" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y135" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z135" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA135" t="s">
+        <v>108</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:T2165">
+  <autoFilter ref="A1:T2169">
     <sortState ref="A2:T111">
-      <sortCondition ref="A1:A2165"/>
+      <sortCondition ref="A1:A2169"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update with latest info from SAP note ; 1928533
</commit_message>
<xml_diff>
--- a/AzureVMSizes.xlsx
+++ b/AzureVMSizes.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karim\Documents\sourcetree\azure-vmchooser-database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kavaes\Documents\SourceTree\azure-vmchooser-database\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10095"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10092"/>
   </bookViews>
   <sheets>
     <sheet name="AzureVMSizes" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1358" uniqueCount="178">
   <si>
     <t>Name</t>
   </si>
@@ -553,6 +553,9 @@
   </si>
   <si>
     <t>Standard_D64s_v3</t>
+  </si>
+  <si>
+    <t>Supported</t>
   </si>
 </sst>
 </file>
@@ -1074,25 +1077,25 @@
     <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Berekening" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Controlecel" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Gekoppelde cel" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Goed" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Invoer" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Komma" xfId="42" builtinId="3"/>
-    <cellStyle name="Kop 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Kop 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Kop 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Kop 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Neutraal" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notitie" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Ongeldig" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
-    <cellStyle name="Titel" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Totaal" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Uitvoer" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Verklarende tekst" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Waarschuwingstekst" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Comma" xfId="42" builtinId="3"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1108,9 +1111,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1148,7 +1151,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1254,7 +1257,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1407,43 +1410,43 @@
   <dimension ref="A1:AA135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2670" ySplit="570" topLeftCell="A109" activePane="bottomRight"/>
+      <pane xSplit="2676" ySplit="576" topLeftCell="Q124" activePane="bottomRight"/>
       <selection sqref="A1:A1048576"/>
       <selection pane="topRight" activeCell="AA1" sqref="AA1"/>
       <selection pane="bottomLeft" activeCell="A129" sqref="A129"/>
-      <selection pane="bottomRight" activeCell="K107" sqref="K107"/>
+      <selection pane="bottomRight" activeCell="Z16" sqref="Z16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1526,7 +1529,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1618,7 +1621,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1709,7 +1712,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1800,7 +1803,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1891,7 +1894,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1982,7 +1985,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>132</v>
       </c>
@@ -2072,13 +2075,13 @@
         <v>143</v>
       </c>
       <c r="Z7" s="1" t="s">
-        <v>143</v>
+        <v>177</v>
       </c>
       <c r="AA7" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>133</v>
       </c>
@@ -2168,13 +2171,13 @@
         <v>143</v>
       </c>
       <c r="Z8" s="1" t="s">
-        <v>143</v>
+        <v>177</v>
       </c>
       <c r="AA8" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>134</v>
       </c>
@@ -2264,13 +2267,13 @@
         <v>143</v>
       </c>
       <c r="Z9" s="1" t="s">
-        <v>143</v>
+        <v>177</v>
       </c>
       <c r="AA9" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>135</v>
       </c>
@@ -2360,13 +2363,13 @@
         <v>143</v>
       </c>
       <c r="Z10" s="1" t="s">
-        <v>143</v>
+        <v>177</v>
       </c>
       <c r="AA10" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>136</v>
       </c>
@@ -2456,13 +2459,13 @@
         <v>143</v>
       </c>
       <c r="Z11" s="1" t="s">
-        <v>143</v>
+        <v>177</v>
       </c>
       <c r="AA11" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>138</v>
       </c>
@@ -2552,13 +2555,13 @@
         <v>143</v>
       </c>
       <c r="Z12" s="1" t="s">
-        <v>143</v>
+        <v>177</v>
       </c>
       <c r="AA12" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>127</v>
       </c>
@@ -2648,13 +2651,13 @@
         <v>143</v>
       </c>
       <c r="Z13" s="1" t="s">
-        <v>143</v>
+        <v>177</v>
       </c>
       <c r="AA13" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>131</v>
       </c>
@@ -2744,13 +2747,13 @@
         <v>143</v>
       </c>
       <c r="Z14" s="1" t="s">
-        <v>143</v>
+        <v>177</v>
       </c>
       <c r="AA14" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>137</v>
       </c>
@@ -2840,13 +2843,13 @@
         <v>143</v>
       </c>
       <c r="Z15" s="1" t="s">
-        <v>143</v>
+        <v>177</v>
       </c>
       <c r="AA15" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>139</v>
       </c>
@@ -2936,13 +2939,13 @@
         <v>143</v>
       </c>
       <c r="Z16" s="1" t="s">
-        <v>143</v>
+        <v>177</v>
       </c>
       <c r="AA16" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -3034,7 +3037,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -3125,7 +3128,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>56</v>
       </c>
@@ -3216,7 +3219,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>100</v>
       </c>
@@ -3294,8 +3297,8 @@
       <c r="W20" s="1">
         <v>46</v>
       </c>
-      <c r="X20" s="1" t="s">
-        <v>143</v>
+      <c r="X20" s="1">
+        <v>11000</v>
       </c>
       <c r="Y20" s="1" t="s">
         <v>143</v>
@@ -3307,7 +3310,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>101</v>
       </c>
@@ -3385,8 +3388,8 @@
       <c r="W21" s="1">
         <v>93</v>
       </c>
-      <c r="X21" s="1" t="s">
-        <v>143</v>
+      <c r="X21" s="1">
+        <v>22000</v>
       </c>
       <c r="Y21" s="1" t="s">
         <v>143</v>
@@ -3398,7 +3401,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -3489,7 +3492,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>58</v>
       </c>
@@ -3580,7 +3583,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -3671,7 +3674,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -3762,7 +3765,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -3853,7 +3856,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>60</v>
       </c>
@@ -3931,11 +3934,11 @@
       <c r="W27" s="1">
         <v>93</v>
       </c>
-      <c r="X27" s="1">
-        <v>30430</v>
+      <c r="X27" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="Y27" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="Z27" s="1" t="s">
         <v>143</v>
@@ -3944,7 +3947,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>59</v>
       </c>
@@ -4035,7 +4038,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>23</v>
       </c>
@@ -4114,10 +4117,10 @@
         <v>375</v>
       </c>
       <c r="X29" s="1">
-        <v>6680</v>
-      </c>
-      <c r="Y29" s="1" t="s">
-        <v>144</v>
+        <v>1500</v>
+      </c>
+      <c r="Y29" s="1">
+        <v>12000</v>
       </c>
       <c r="Z29" s="1" t="s">
         <v>143</v>
@@ -4126,7 +4129,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -4204,11 +4207,11 @@
       <c r="W30" s="1">
         <v>10</v>
       </c>
-      <c r="X30" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="Y30" s="1" t="s">
-        <v>143</v>
+      <c r="X30" s="1">
+        <v>3000</v>
+      </c>
+      <c r="Y30" s="1">
+        <v>25000</v>
       </c>
       <c r="Z30" s="1" t="s">
         <v>143</v>
@@ -4217,7 +4220,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>25</v>
       </c>
@@ -4296,10 +4299,10 @@
         <v>20</v>
       </c>
       <c r="X31" s="1">
-        <v>24180</v>
-      </c>
-      <c r="Y31" s="1" t="s">
-        <v>144</v>
+        <v>6000</v>
+      </c>
+      <c r="Y31" s="1">
+        <v>50000</v>
       </c>
       <c r="Z31" s="1" t="s">
         <v>143</v>
@@ -4308,7 +4311,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>98</v>
       </c>
@@ -4386,8 +4389,8 @@
       <c r="W32" s="1">
         <v>20</v>
       </c>
-      <c r="X32" s="1" t="s">
-        <v>143</v>
+      <c r="X32" s="1">
+        <v>11000</v>
       </c>
       <c r="Y32" s="1" t="s">
         <v>143</v>
@@ -4399,7 +4402,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>62</v>
       </c>
@@ -4477,11 +4480,11 @@
       <c r="W33" s="1">
         <v>40</v>
       </c>
-      <c r="X33" s="1">
-        <v>12300</v>
+      <c r="X33" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="Y33" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="Z33" s="1" t="s">
         <v>143</v>
@@ -4490,7 +4493,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>61</v>
       </c>
@@ -4581,7 +4584,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>99</v>
       </c>
@@ -4660,10 +4663,10 @@
         <v>80</v>
       </c>
       <c r="X35" s="1">
-        <v>3530</v>
+        <v>22000</v>
       </c>
       <c r="Y35" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="Z35" s="1" t="s">
         <v>143</v>
@@ -4672,7 +4675,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>63</v>
       </c>
@@ -4763,7 +4766,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>26</v>
       </c>
@@ -4854,7 +4857,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>67</v>
       </c>
@@ -4932,11 +4935,11 @@
       <c r="W38" s="1">
         <v>46</v>
       </c>
-      <c r="X38" s="1" t="s">
-        <v>143</v>
+      <c r="X38" s="1">
+        <v>2325</v>
       </c>
       <c r="Y38" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="Z38" s="1" t="s">
         <v>143</v>
@@ -4945,7 +4948,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>31</v>
       </c>
@@ -5036,7 +5039,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>68</v>
       </c>
@@ -5115,10 +5118,10 @@
         <v>187</v>
       </c>
       <c r="X40" s="1">
-        <v>22000</v>
+        <v>4650</v>
       </c>
       <c r="Y40" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="Z40" s="1" t="s">
         <v>143</v>
@@ -5127,7 +5130,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>32</v>
       </c>
@@ -5205,8 +5208,8 @@
       <c r="W41" s="1">
         <v>46</v>
       </c>
-      <c r="X41" s="1">
-        <v>11000</v>
+      <c r="X41" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="Y41" s="1" t="s">
         <v>143</v>
@@ -5218,7 +5221,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>69</v>
       </c>
@@ -5296,8 +5299,8 @@
       <c r="W42" s="1">
         <v>93</v>
       </c>
-      <c r="X42" s="1" t="s">
-        <v>143</v>
+      <c r="X42" s="1">
+        <v>9300</v>
       </c>
       <c r="Y42" s="1" t="s">
         <v>143</v>
@@ -5309,7 +5312,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>33</v>
       </c>
@@ -5400,7 +5403,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>70</v>
       </c>
@@ -5478,8 +5481,8 @@
       <c r="W44" s="1">
         <v>375</v>
       </c>
-      <c r="X44" s="1" t="s">
-        <v>143</v>
+      <c r="X44" s="1">
+        <v>18600</v>
       </c>
       <c r="Y44" s="1" t="s">
         <v>143</v>
@@ -5491,7 +5494,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>34</v>
       </c>
@@ -5582,7 +5585,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>35</v>
       </c>
@@ -5673,7 +5676,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>64</v>
       </c>
@@ -5764,7 +5767,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>27</v>
       </c>
@@ -5855,7 +5858,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>65</v>
       </c>
@@ -5946,7 +5949,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>28</v>
       </c>
@@ -6037,7 +6040,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>66</v>
       </c>
@@ -6128,7 +6131,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>29</v>
       </c>
@@ -6219,7 +6222,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>30</v>
       </c>
@@ -6310,7 +6313,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>15</v>
       </c>
@@ -6399,7 +6402,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>41</v>
       </c>
@@ -6488,7 +6491,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>19</v>
       </c>
@@ -6564,11 +6567,11 @@
       <c r="W56" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="X56" s="1" t="s">
-        <v>143</v>
+      <c r="X56" s="1">
+        <v>2325</v>
       </c>
       <c r="Y56" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="Z56" s="1" t="s">
         <v>143</v>
@@ -6577,7 +6580,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="57" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>46</v>
       </c>
@@ -6653,11 +6656,11 @@
       <c r="W57" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="X57" s="1" t="s">
-        <v>143</v>
+      <c r="X57" s="1">
+        <v>3530</v>
       </c>
       <c r="Y57" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="Z57" s="1" t="s">
         <v>143</v>
@@ -6666,7 +6669,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="58" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>20</v>
       </c>
@@ -6742,11 +6745,11 @@
       <c r="W58" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="X58" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="Y58" s="1" t="s">
-        <v>143</v>
+      <c r="X58" s="1">
+        <v>4650</v>
+      </c>
+      <c r="Y58" s="1">
+        <v>48750</v>
       </c>
       <c r="Z58" s="1" t="s">
         <v>143</v>
@@ -6755,7 +6758,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="59" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>47</v>
       </c>
@@ -6831,11 +6834,11 @@
       <c r="W59" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="X59" s="1" t="s">
-        <v>143</v>
+      <c r="X59" s="1">
+        <v>6680</v>
       </c>
       <c r="Y59" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="Z59" s="1" t="s">
         <v>143</v>
@@ -6844,7 +6847,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="60" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>21</v>
       </c>
@@ -6920,11 +6923,11 @@
       <c r="W60" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="X60" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="Y60" s="1" t="s">
-        <v>143</v>
+      <c r="X60" s="1">
+        <v>9300</v>
+      </c>
+      <c r="Y60" s="1">
+        <v>91050</v>
       </c>
       <c r="Z60" s="1" t="s">
         <v>143</v>
@@ -6933,7 +6936,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="61" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>48</v>
       </c>
@@ -7010,10 +7013,10 @@
         <v>120</v>
       </c>
       <c r="X61" s="1">
-        <v>22000</v>
+        <v>12300</v>
       </c>
       <c r="Y61" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="Z61" s="1" t="s">
         <v>143</v>
@@ -7022,7 +7025,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="62" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>22</v>
       </c>
@@ -7099,10 +7102,10 @@
         <v>120</v>
       </c>
       <c r="X62" s="1">
-        <v>11000</v>
+        <v>18600</v>
       </c>
       <c r="Y62" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="Z62" s="1" t="s">
         <v>143</v>
@@ -7111,7 +7114,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="63" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>49</v>
       </c>
@@ -7187,11 +7190,11 @@
       <c r="W63" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="X63" s="1" t="s">
-        <v>143</v>
+      <c r="X63" s="1">
+        <v>24180</v>
       </c>
       <c r="Y63" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="Z63" s="1" t="s">
         <v>143</v>
@@ -7200,7 +7203,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="64" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>50</v>
       </c>
@@ -7276,11 +7279,11 @@
       <c r="W64" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="X64" s="1" t="s">
-        <v>143</v>
+      <c r="X64" s="1">
+        <v>30430</v>
       </c>
       <c r="Y64" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="Z64" s="1" t="s">
         <v>143</v>
@@ -7289,7 +7292,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="65" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>16</v>
       </c>
@@ -7378,7 +7381,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="66" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>42</v>
       </c>
@@ -7467,7 +7470,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="67" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>17</v>
       </c>
@@ -7556,7 +7559,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="68" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>43</v>
       </c>
@@ -7645,7 +7648,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="69" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>18</v>
       </c>
@@ -7734,7 +7737,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="70" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>44</v>
       </c>
@@ -7823,7 +7826,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="71" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>45</v>
       </c>
@@ -7912,7 +7915,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="72" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>36</v>
       </c>
@@ -8003,7 +8006,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="73" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>40</v>
       </c>
@@ -8094,7 +8097,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="74" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>55</v>
       </c>
@@ -8183,7 +8186,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="75" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>51</v>
       </c>
@@ -8272,7 +8275,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="76" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>37</v>
       </c>
@@ -8363,7 +8366,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="77" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>52</v>
       </c>
@@ -8452,7 +8455,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="78" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>38</v>
       </c>
@@ -8543,7 +8546,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="79" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>53</v>
       </c>
@@ -8632,7 +8635,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="80" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>39</v>
       </c>
@@ -8723,7 +8726,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>54</v>
       </c>
@@ -8812,7 +8815,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>74</v>
       </c>
@@ -8903,7 +8906,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>75</v>
       </c>
@@ -8981,8 +8984,8 @@
       <c r="W83" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="X83" s="1">
-        <v>41670</v>
+      <c r="X83" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="Y83" s="1" t="s">
         <v>144</v>
@@ -8994,7 +8997,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="84" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>76</v>
       </c>
@@ -9085,7 +9088,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="85" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>77</v>
       </c>
@@ -9163,8 +9166,8 @@
       <c r="W85" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="X85" s="1">
-        <v>22680</v>
+      <c r="X85" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="Y85" s="1" t="s">
         <v>143</v>
@@ -9176,7 +9179,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="86" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>78</v>
       </c>
@@ -9267,7 +9270,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>79</v>
       </c>
@@ -9344,10 +9347,10 @@
         <v>120</v>
       </c>
       <c r="X87" s="1">
-        <v>11870</v>
-      </c>
-      <c r="Y87" s="1" t="s">
-        <v>143</v>
+        <v>3580</v>
+      </c>
+      <c r="Y87" s="1">
+        <v>34415</v>
       </c>
       <c r="Z87" s="1" t="s">
         <v>143</v>
@@ -9356,7 +9359,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="88" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>80</v>
       </c>
@@ -9432,11 +9435,11 @@
       <c r="W88" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="X88" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="Y88" s="1" t="s">
-        <v>143</v>
+      <c r="X88" s="1">
+        <v>6900</v>
+      </c>
+      <c r="Y88" s="1">
+        <v>78620</v>
       </c>
       <c r="Z88" s="1" t="s">
         <v>143</v>
@@ -9445,7 +9448,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>81</v>
       </c>
@@ -9522,10 +9525,10 @@
         <v>120</v>
       </c>
       <c r="X89" s="1">
-        <v>6900</v>
-      </c>
-      <c r="Y89" s="1" t="s">
-        <v>143</v>
+        <v>11870</v>
+      </c>
+      <c r="Y89" s="1">
+        <v>137520</v>
       </c>
       <c r="Z89" s="1" t="s">
         <v>143</v>
@@ -9534,7 +9537,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="90" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>82</v>
       </c>
@@ -9610,11 +9613,11 @@
       <c r="W90" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="X90" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="Y90" s="1" t="s">
-        <v>143</v>
+      <c r="X90" s="1">
+        <v>22680</v>
+      </c>
+      <c r="Y90" s="1">
+        <v>247880</v>
       </c>
       <c r="Z90" s="1" t="s">
         <v>143</v>
@@ -9623,7 +9626,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="91" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>83</v>
       </c>
@@ -9700,10 +9703,10 @@
         <v>120</v>
       </c>
       <c r="X91" s="1">
-        <v>3580</v>
+        <v>41670</v>
       </c>
       <c r="Y91" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="Z91" s="1" t="s">
         <v>143</v>
@@ -9712,7 +9715,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="92" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>89</v>
       </c>
@@ -9803,7 +9806,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="93" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>91</v>
       </c>
@@ -9894,7 +9897,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="94" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>93</v>
       </c>
@@ -9985,7 +9988,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="95" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>92</v>
       </c>
@@ -10076,7 +10079,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="96" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>88</v>
       </c>
@@ -10167,7 +10170,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="97" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>90</v>
       </c>
@@ -10258,7 +10261,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="98" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>86</v>
       </c>
@@ -10347,7 +10350,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="99" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>87</v>
       </c>
@@ -10436,7 +10439,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="100" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>84</v>
       </c>
@@ -10525,7 +10528,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="101" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>85</v>
       </c>
@@ -10614,7 +10617,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="102" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>126</v>
       </c>
@@ -10689,26 +10692,23 @@
         <f t="shared" si="37"/>
         <v>100</v>
       </c>
-      <c r="W102" s="2">
-        <f t="shared" si="37"/>
-        <v>40960000</v>
-      </c>
-      <c r="X102" s="2">
-        <f t="shared" ref="X102:X111" si="38">IFERROR(T102/W102*1000,"Unknown")</f>
-        <v>9.765625E-2</v>
-      </c>
-      <c r="Y102" s="2">
-        <f t="shared" ref="Y102:Y111" si="39">IFERROR(U102/X102*1000,"Unknown")</f>
-        <v>204800000</v>
+      <c r="W102" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="X102" s="1">
+        <v>134630</v>
+      </c>
+      <c r="Y102" s="1" t="s">
+        <v>144</v>
       </c>
       <c r="Z102" s="1" t="s">
-        <v>109</v>
+        <v>143</v>
       </c>
       <c r="AA102" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="103" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>103</v>
       </c>
@@ -10783,26 +10783,23 @@
         <f t="shared" si="37"/>
         <v>100</v>
       </c>
-      <c r="W103" s="2">
-        <f t="shared" si="37"/>
-        <v>40960000</v>
-      </c>
-      <c r="X103" s="2">
-        <f t="shared" si="38"/>
-        <v>9.765625E-2</v>
-      </c>
-      <c r="Y103" s="2">
-        <f t="shared" si="39"/>
-        <v>204800000</v>
+      <c r="W103" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="X103" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y103" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="Z103" s="1" t="s">
-        <v>109</v>
+        <v>143</v>
       </c>
       <c r="AA103" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="104" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>102</v>
       </c>
@@ -10877,26 +10874,23 @@
         <f t="shared" si="37"/>
         <v>50</v>
       </c>
-      <c r="W104" s="2">
-        <f t="shared" si="37"/>
-        <v>40960000</v>
-      </c>
-      <c r="X104" s="2">
-        <f t="shared" si="38"/>
-        <v>4.8828125E-2</v>
-      </c>
-      <c r="Y104" s="2">
-        <f t="shared" si="39"/>
-        <v>409600000</v>
+      <c r="W104" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="X104" s="1">
+        <v>68930</v>
+      </c>
+      <c r="Y104" s="1" t="s">
+        <v>144</v>
       </c>
       <c r="Z104" s="1" t="s">
-        <v>109</v>
+        <v>143</v>
       </c>
       <c r="AA104" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="105" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>95</v>
       </c>
@@ -10943,19 +10937,19 @@
         <v>196608</v>
       </c>
       <c r="O105">
-        <f t="shared" ref="O105:O111" si="40">500*$M105</f>
+        <f t="shared" ref="O105:O111" si="38">500*$M105</f>
         <v>24000</v>
       </c>
       <c r="P105">
-        <f t="shared" ref="P105:P111" si="41">60*$M105</f>
+        <f t="shared" ref="P105:P111" si="39">60*$M105</f>
         <v>2880</v>
       </c>
       <c r="Q105">
-        <f t="shared" ref="Q105:R111" si="42">O105</f>
+        <f t="shared" ref="Q105:R111" si="40">O105</f>
         <v>24000</v>
       </c>
       <c r="R105">
-        <f t="shared" si="42"/>
+        <f t="shared" si="40"/>
         <v>2880</v>
       </c>
       <c r="S105">
@@ -10973,26 +10967,23 @@
         <f t="shared" si="37"/>
         <v>81.599999999999994</v>
       </c>
-      <c r="W105" s="2">
-        <f t="shared" si="37"/>
-        <v>8533333.333333334</v>
-      </c>
-      <c r="X105" s="2">
-        <f t="shared" si="38"/>
-        <v>7.9687499999999994E-2</v>
-      </c>
-      <c r="Y105" s="2">
-        <f t="shared" si="39"/>
-        <v>442906574.39446372</v>
+      <c r="W105" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="X105" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y105" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="Z105" s="1" t="s">
-        <v>109</v>
+        <v>143</v>
       </c>
       <c r="AA105" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="106" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>96</v>
       </c>
@@ -11039,19 +11030,19 @@
         <v>262144</v>
       </c>
       <c r="O106">
+        <f t="shared" si="38"/>
+        <v>32000</v>
+      </c>
+      <c r="P106">
+        <f t="shared" si="39"/>
+        <v>3840</v>
+      </c>
+      <c r="Q106">
         <f t="shared" si="40"/>
         <v>32000</v>
       </c>
-      <c r="P106">
-        <f t="shared" si="41"/>
-        <v>3840</v>
-      </c>
-      <c r="Q106">
-        <f t="shared" si="42"/>
-        <v>32000</v>
-      </c>
       <c r="R106">
-        <f t="shared" si="42"/>
+        <f t="shared" si="40"/>
         <v>3840</v>
       </c>
       <c r="S106">
@@ -11069,26 +11060,23 @@
         <f t="shared" si="37"/>
         <v>172.8</v>
       </c>
-      <c r="W106" s="2">
-        <f t="shared" si="37"/>
-        <v>8533333.3333333321</v>
-      </c>
-      <c r="X106" s="2">
-        <f t="shared" si="38"/>
-        <v>0.16875000000000004</v>
-      </c>
-      <c r="Y106" s="2">
-        <f t="shared" si="39"/>
-        <v>131687242.7983539</v>
+      <c r="W106" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="X106" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y106" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="Z106" s="1" t="s">
-        <v>109</v>
+        <v>143</v>
       </c>
       <c r="AA106" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="107" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>97</v>
       </c>
@@ -11135,19 +11123,19 @@
         <v>262144</v>
       </c>
       <c r="O107">
+        <f t="shared" si="38"/>
+        <v>32000</v>
+      </c>
+      <c r="P107">
+        <f t="shared" si="39"/>
+        <v>3840</v>
+      </c>
+      <c r="Q107">
         <f t="shared" si="40"/>
         <v>32000</v>
       </c>
-      <c r="P107">
-        <f t="shared" si="41"/>
-        <v>3840</v>
-      </c>
-      <c r="Q107">
-        <f t="shared" si="42"/>
-        <v>32000</v>
-      </c>
       <c r="R107">
-        <f t="shared" si="42"/>
+        <f t="shared" si="40"/>
         <v>3840</v>
       </c>
       <c r="S107">
@@ -11165,26 +11153,23 @@
         <f t="shared" si="37"/>
         <v>172.8</v>
       </c>
-      <c r="W107" s="2">
-        <f t="shared" si="37"/>
-        <v>8533333.3333333321</v>
-      </c>
-      <c r="X107" s="2">
-        <f t="shared" si="38"/>
-        <v>0.16875000000000004</v>
-      </c>
-      <c r="Y107" s="2">
-        <f t="shared" si="39"/>
-        <v>131687242.7983539</v>
+      <c r="W107" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="X107" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y107" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="Z107" s="1" t="s">
-        <v>109</v>
+        <v>143</v>
       </c>
       <c r="AA107" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="108" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>94</v>
       </c>
@@ -11231,19 +11216,19 @@
         <v>98304</v>
       </c>
       <c r="O108">
+        <f t="shared" si="38"/>
+        <v>12000</v>
+      </c>
+      <c r="P108">
+        <f t="shared" si="39"/>
+        <v>1440</v>
+      </c>
+      <c r="Q108">
         <f t="shared" si="40"/>
         <v>12000</v>
       </c>
-      <c r="P108">
-        <f t="shared" si="41"/>
-        <v>1440</v>
-      </c>
-      <c r="Q108">
-        <f t="shared" si="42"/>
-        <v>12000</v>
-      </c>
       <c r="R108">
-        <f t="shared" si="42"/>
+        <f t="shared" si="40"/>
         <v>1440</v>
       </c>
       <c r="S108">
@@ -11261,26 +11246,23 @@
         <f t="shared" si="37"/>
         <v>45.6</v>
       </c>
-      <c r="W108" s="2">
-        <f t="shared" si="37"/>
-        <v>8533333.333333334</v>
-      </c>
-      <c r="X108" s="2">
-        <f t="shared" si="38"/>
-        <v>4.4531249999999994E-2</v>
-      </c>
-      <c r="Y108" s="2">
-        <f t="shared" si="39"/>
-        <v>709141274.23822713</v>
+      <c r="W108" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="X108" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y108" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="Z108" s="1" t="s">
-        <v>109</v>
+        <v>143</v>
       </c>
       <c r="AA108" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="109" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>72</v>
       </c>
@@ -11327,19 +11309,19 @@
         <v>196608</v>
       </c>
       <c r="O109">
+        <f t="shared" si="38"/>
+        <v>24000</v>
+      </c>
+      <c r="P109">
+        <f t="shared" si="39"/>
+        <v>2880</v>
+      </c>
+      <c r="Q109">
         <f t="shared" si="40"/>
         <v>24000</v>
       </c>
-      <c r="P109">
-        <f t="shared" si="41"/>
-        <v>2880</v>
-      </c>
-      <c r="Q109">
-        <f t="shared" si="42"/>
-        <v>24000</v>
-      </c>
       <c r="R109">
-        <f t="shared" si="42"/>
+        <f t="shared" si="40"/>
         <v>2880</v>
       </c>
       <c r="S109">
@@ -11357,26 +11339,23 @@
         <f t="shared" si="37"/>
         <v>81.599999999999994</v>
       </c>
-      <c r="W109" s="2">
-        <f t="shared" si="37"/>
-        <v>8533333.333333334</v>
-      </c>
-      <c r="X109" s="2">
-        <f t="shared" si="38"/>
-        <v>7.9687499999999994E-2</v>
-      </c>
-      <c r="Y109" s="2">
-        <f t="shared" si="39"/>
-        <v>442906574.39446372</v>
+      <c r="W109" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="X109" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y109" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="Z109" s="1" t="s">
-        <v>109</v>
+        <v>143</v>
       </c>
       <c r="AA109" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>73</v>
       </c>
@@ -11423,19 +11402,19 @@
         <v>262144</v>
       </c>
       <c r="O110">
+        <f t="shared" si="38"/>
+        <v>32000</v>
+      </c>
+      <c r="P110">
+        <f t="shared" si="39"/>
+        <v>3840</v>
+      </c>
+      <c r="Q110">
         <f t="shared" si="40"/>
         <v>32000</v>
       </c>
-      <c r="P110">
-        <f t="shared" si="41"/>
-        <v>3840</v>
-      </c>
-      <c r="Q110">
-        <f t="shared" si="42"/>
-        <v>32000</v>
-      </c>
       <c r="R110">
-        <f t="shared" si="42"/>
+        <f t="shared" si="40"/>
         <v>3840</v>
       </c>
       <c r="S110">
@@ -11453,26 +11432,23 @@
         <f t="shared" si="37"/>
         <v>172.8</v>
       </c>
-      <c r="W110" s="2">
-        <f t="shared" si="37"/>
-        <v>8533333.3333333321</v>
-      </c>
-      <c r="X110" s="2">
-        <f t="shared" si="38"/>
-        <v>0.16875000000000004</v>
-      </c>
-      <c r="Y110" s="2">
-        <f t="shared" si="39"/>
-        <v>131687242.7983539</v>
+      <c r="W110" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="X110" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y110" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="Z110" s="1" t="s">
-        <v>109</v>
+        <v>143</v>
       </c>
       <c r="AA110" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="111" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>71</v>
       </c>
@@ -11519,19 +11495,19 @@
         <v>98304</v>
       </c>
       <c r="O111">
+        <f t="shared" si="38"/>
+        <v>12000</v>
+      </c>
+      <c r="P111">
+        <f t="shared" si="39"/>
+        <v>1440</v>
+      </c>
+      <c r="Q111">
         <f t="shared" si="40"/>
         <v>12000</v>
       </c>
-      <c r="P111">
-        <f t="shared" si="41"/>
-        <v>1440</v>
-      </c>
-      <c r="Q111">
-        <f t="shared" si="42"/>
-        <v>12000</v>
-      </c>
       <c r="R111">
-        <f t="shared" si="42"/>
+        <f t="shared" si="40"/>
         <v>1440</v>
       </c>
       <c r="S111">
@@ -11549,26 +11525,23 @@
         <f t="shared" si="37"/>
         <v>45.6</v>
       </c>
-      <c r="W111" s="2">
-        <f t="shared" si="37"/>
-        <v>8533333.333333334</v>
-      </c>
-      <c r="X111" s="2">
-        <f t="shared" si="38"/>
-        <v>4.4531249999999994E-2</v>
-      </c>
-      <c r="Y111" s="2">
-        <f t="shared" si="39"/>
-        <v>709141274.23822713</v>
+      <c r="W111" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="X111" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y111" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="Z111" s="1" t="s">
-        <v>109</v>
+        <v>143</v>
       </c>
       <c r="AA111" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="112" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>145</v>
       </c>
@@ -11585,11 +11558,11 @@
         <v>120</v>
       </c>
       <c r="F112" s="1" t="str">
-        <f t="shared" ref="F112:F117" si="43">IFERROR(E112*I112,"Unknown")</f>
+        <f t="shared" ref="F112:F117" si="41">IFERROR(E112*I112,"Unknown")</f>
         <v>Unknown</v>
       </c>
       <c r="G112" s="2" t="str">
-        <f t="shared" ref="G112:G117" si="44">IFERROR(C112/F112*1000,"Unknown")</f>
+        <f t="shared" ref="G112:G117" si="42">IFERROR(C112/F112*1000,"Unknown")</f>
         <v>Unknown</v>
       </c>
       <c r="H112" t="s">
@@ -11657,7 +11630,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="113" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>146</v>
       </c>
@@ -11674,11 +11647,11 @@
         <v>120</v>
       </c>
       <c r="F113" s="1" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="41"/>
         <v>Unknown</v>
       </c>
       <c r="G113" s="2" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="42"/>
         <v>Unknown</v>
       </c>
       <c r="H113" t="s">
@@ -11701,15 +11674,15 @@
         <v>8</v>
       </c>
       <c r="N113" s="1">
-        <f t="shared" ref="N113:N127" si="45">M113*4*1024</f>
+        <f t="shared" ref="N113:N127" si="43">M113*4*1024</f>
         <v>32768</v>
       </c>
       <c r="O113" s="1">
-        <f t="shared" ref="O113:O127" si="46">M113*500</f>
+        <f t="shared" ref="O113:O127" si="44">M113*500</f>
         <v>4000</v>
       </c>
       <c r="P113" s="1">
-        <f t="shared" ref="P113:P127" si="47">M113*60</f>
+        <f t="shared" ref="P113:P127" si="45">M113*60</f>
         <v>480</v>
       </c>
       <c r="Q113" s="1">
@@ -11746,7 +11719,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="114" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>147</v>
       </c>
@@ -11763,11 +11736,11 @@
         <v>120</v>
       </c>
       <c r="F114" s="1" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="41"/>
         <v>Unknown</v>
       </c>
       <c r="G114" s="2" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="42"/>
         <v>Unknown</v>
       </c>
       <c r="H114" t="s">
@@ -11790,15 +11763,15 @@
         <v>16</v>
       </c>
       <c r="N114" s="1">
+        <f t="shared" si="43"/>
+        <v>65536</v>
+      </c>
+      <c r="O114" s="1">
+        <f t="shared" si="44"/>
+        <v>8000</v>
+      </c>
+      <c r="P114" s="1">
         <f t="shared" si="45"/>
-        <v>65536</v>
-      </c>
-      <c r="O114" s="1">
-        <f t="shared" si="46"/>
-        <v>8000</v>
-      </c>
-      <c r="P114" s="1">
-        <f t="shared" si="47"/>
         <v>960</v>
       </c>
       <c r="Q114" s="1">
@@ -11835,7 +11808,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="115" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>148</v>
       </c>
@@ -11852,11 +11825,11 @@
         <v>120</v>
       </c>
       <c r="F115" s="1" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="41"/>
         <v>Unknown</v>
       </c>
       <c r="G115" s="2" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="42"/>
         <v>Unknown</v>
       </c>
       <c r="H115" t="s">
@@ -11879,15 +11852,15 @@
         <v>32</v>
       </c>
       <c r="N115" s="1">
+        <f t="shared" si="43"/>
+        <v>131072</v>
+      </c>
+      <c r="O115" s="1">
+        <f t="shared" si="44"/>
+        <v>16000</v>
+      </c>
+      <c r="P115" s="1">
         <f t="shared" si="45"/>
-        <v>131072</v>
-      </c>
-      <c r="O115" s="1">
-        <f t="shared" si="46"/>
-        <v>16000</v>
-      </c>
-      <c r="P115" s="1">
-        <f t="shared" si="47"/>
         <v>1920</v>
       </c>
       <c r="Q115" s="1">
@@ -11924,7 +11897,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="116" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>149</v>
       </c>
@@ -11941,11 +11914,11 @@
         <v>120</v>
       </c>
       <c r="F116" s="1" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="41"/>
         <v>Unknown</v>
       </c>
       <c r="G116" s="2" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="42"/>
         <v>Unknown</v>
       </c>
       <c r="H116" t="s">
@@ -11968,15 +11941,15 @@
         <v>64</v>
       </c>
       <c r="N116" s="1">
+        <f t="shared" si="43"/>
+        <v>262144</v>
+      </c>
+      <c r="O116" s="1">
+        <f t="shared" si="44"/>
+        <v>32000</v>
+      </c>
+      <c r="P116" s="1">
         <f t="shared" si="45"/>
-        <v>262144</v>
-      </c>
-      <c r="O116" s="1">
-        <f t="shared" si="46"/>
-        <v>32000</v>
-      </c>
-      <c r="P116" s="1">
-        <f t="shared" si="47"/>
         <v>3840</v>
       </c>
       <c r="Q116" s="1">
@@ -12013,7 +11986,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="117" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>150</v>
       </c>
@@ -12030,11 +12003,11 @@
         <v>120</v>
       </c>
       <c r="F117" s="1" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="41"/>
         <v>Unknown</v>
       </c>
       <c r="G117" s="2" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="42"/>
         <v>Unknown</v>
       </c>
       <c r="H117" t="s">
@@ -12057,15 +12030,15 @@
         <v>64</v>
       </c>
       <c r="N117" s="1">
+        <f t="shared" si="43"/>
+        <v>262144</v>
+      </c>
+      <c r="O117" s="1">
+        <f t="shared" si="44"/>
+        <v>32000</v>
+      </c>
+      <c r="P117" s="1">
         <f t="shared" si="45"/>
-        <v>262144</v>
-      </c>
-      <c r="O117" s="1">
-        <f t="shared" si="46"/>
-        <v>32000</v>
-      </c>
-      <c r="P117" s="1">
-        <f t="shared" si="47"/>
         <v>3840</v>
       </c>
       <c r="Q117" s="1">
@@ -12102,7 +12075,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="118" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>168</v>
       </c>
@@ -12119,11 +12092,11 @@
         <v>120</v>
       </c>
       <c r="F118" s="1" t="str">
-        <f t="shared" ref="F118:F127" si="48">IFERROR(E118*I118,"Unknown")</f>
+        <f t="shared" ref="F118:F127" si="46">IFERROR(E118*I118,"Unknown")</f>
         <v>Unknown</v>
       </c>
       <c r="G118" s="2" t="str">
-        <f t="shared" ref="G118:G127" si="49">IFERROR(C118/F118*1000,"Unknown")</f>
+        <f t="shared" ref="G118:G127" si="47">IFERROR(C118/F118*1000,"Unknown")</f>
         <v>Unknown</v>
       </c>
       <c r="H118" t="s">
@@ -12146,15 +12119,15 @@
         <v>4</v>
       </c>
       <c r="N118" s="1">
+        <f t="shared" si="43"/>
+        <v>16384</v>
+      </c>
+      <c r="O118" s="1">
+        <f t="shared" si="44"/>
+        <v>2000</v>
+      </c>
+      <c r="P118" s="1">
         <f t="shared" si="45"/>
-        <v>16384</v>
-      </c>
-      <c r="O118" s="1">
-        <f t="shared" si="46"/>
-        <v>2000</v>
-      </c>
-      <c r="P118" s="1">
-        <f t="shared" si="47"/>
         <v>240</v>
       </c>
       <c r="Q118">
@@ -12192,7 +12165,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="119" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>155</v>
       </c>
@@ -12209,11 +12182,11 @@
         <v>120</v>
       </c>
       <c r="F119" s="1" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="46"/>
         <v>Unknown</v>
       </c>
       <c r="G119" s="2" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="47"/>
         <v>Unknown</v>
       </c>
       <c r="H119" t="s">
@@ -12236,15 +12209,15 @@
         <v>8</v>
       </c>
       <c r="N119" s="1">
+        <f t="shared" si="43"/>
+        <v>32768</v>
+      </c>
+      <c r="O119" s="1">
+        <f t="shared" si="44"/>
+        <v>4000</v>
+      </c>
+      <c r="P119" s="1">
         <f t="shared" si="45"/>
-        <v>32768</v>
-      </c>
-      <c r="O119" s="1">
-        <f t="shared" si="46"/>
-        <v>4000</v>
-      </c>
-      <c r="P119" s="1">
-        <f t="shared" si="47"/>
         <v>480</v>
       </c>
       <c r="Q119">
@@ -12282,7 +12255,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="120" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>156</v>
       </c>
@@ -12299,11 +12272,11 @@
         <v>120</v>
       </c>
       <c r="F120" s="1" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="46"/>
         <v>Unknown</v>
       </c>
       <c r="G120" s="2" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="47"/>
         <v>Unknown</v>
       </c>
       <c r="H120" t="s">
@@ -12326,15 +12299,15 @@
         <v>16</v>
       </c>
       <c r="N120" s="1">
+        <f t="shared" si="43"/>
+        <v>65536</v>
+      </c>
+      <c r="O120" s="1">
+        <f t="shared" si="44"/>
+        <v>8000</v>
+      </c>
+      <c r="P120" s="1">
         <f t="shared" si="45"/>
-        <v>65536</v>
-      </c>
-      <c r="O120" s="1">
-        <f t="shared" si="46"/>
-        <v>8000</v>
-      </c>
-      <c r="P120" s="1">
-        <f t="shared" si="47"/>
         <v>960</v>
       </c>
       <c r="Q120">
@@ -12372,7 +12345,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="121" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>157</v>
       </c>
@@ -12389,11 +12362,11 @@
         <v>120</v>
       </c>
       <c r="F121" s="1" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="46"/>
         <v>Unknown</v>
       </c>
       <c r="G121" s="2" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="47"/>
         <v>Unknown</v>
       </c>
       <c r="H121" t="s">
@@ -12416,15 +12389,15 @@
         <v>32</v>
       </c>
       <c r="N121" s="1">
+        <f t="shared" si="43"/>
+        <v>131072</v>
+      </c>
+      <c r="O121" s="1">
+        <f t="shared" si="44"/>
+        <v>16000</v>
+      </c>
+      <c r="P121" s="1">
         <f t="shared" si="45"/>
-        <v>131072</v>
-      </c>
-      <c r="O121" s="1">
-        <f t="shared" si="46"/>
-        <v>16000</v>
-      </c>
-      <c r="P121" s="1">
-        <f t="shared" si="47"/>
         <v>1920</v>
       </c>
       <c r="Q121">
@@ -12462,7 +12435,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="122" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>173</v>
       </c>
@@ -12479,11 +12452,11 @@
         <v>120</v>
       </c>
       <c r="F122" s="1" t="str">
-        <f t="shared" ref="F122:F123" si="50">IFERROR(E122*I122,"Unknown")</f>
+        <f t="shared" ref="F122:F123" si="48">IFERROR(E122*I122,"Unknown")</f>
         <v>Unknown</v>
       </c>
       <c r="G122" s="2" t="str">
-        <f t="shared" ref="G122:G123" si="51">IFERROR(C122/F122*1000,"Unknown")</f>
+        <f t="shared" ref="G122:G123" si="49">IFERROR(C122/F122*1000,"Unknown")</f>
         <v>Unknown</v>
       </c>
       <c r="H122" t="s">
@@ -12548,7 +12521,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="123" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>174</v>
       </c>
@@ -12565,11 +12538,11 @@
         <v>120</v>
       </c>
       <c r="F123" s="1" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="48"/>
         <v>Unknown</v>
       </c>
       <c r="G123" s="2" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="49"/>
         <v>Unknown</v>
       </c>
       <c r="H123" t="s">
@@ -12634,7 +12607,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="124" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>158</v>
       </c>
@@ -12651,11 +12624,11 @@
         <v>120</v>
       </c>
       <c r="F124" s="1" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="46"/>
         <v>Unknown</v>
       </c>
       <c r="G124" s="2" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="47"/>
         <v>Unknown</v>
       </c>
       <c r="H124" t="s">
@@ -12678,15 +12651,15 @@
         <v>4</v>
       </c>
       <c r="N124" s="1">
+        <f t="shared" si="43"/>
+        <v>16384</v>
+      </c>
+      <c r="O124" s="1">
+        <f t="shared" si="44"/>
+        <v>2000</v>
+      </c>
+      <c r="P124" s="1">
         <f t="shared" si="45"/>
-        <v>16384</v>
-      </c>
-      <c r="O124" s="1">
-        <f t="shared" si="46"/>
-        <v>2000</v>
-      </c>
-      <c r="P124" s="1">
-        <f t="shared" si="47"/>
         <v>240</v>
       </c>
       <c r="Q124">
@@ -12723,7 +12696,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="125" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>159</v>
       </c>
@@ -12740,11 +12713,11 @@
         <v>120</v>
       </c>
       <c r="F125" s="1" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="46"/>
         <v>Unknown</v>
       </c>
       <c r="G125" s="2" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="47"/>
         <v>Unknown</v>
       </c>
       <c r="H125" t="s">
@@ -12767,15 +12740,15 @@
         <v>8</v>
       </c>
       <c r="N125" s="1">
+        <f t="shared" si="43"/>
+        <v>32768</v>
+      </c>
+      <c r="O125" s="1">
+        <f t="shared" si="44"/>
+        <v>4000</v>
+      </c>
+      <c r="P125" s="1">
         <f t="shared" si="45"/>
-        <v>32768</v>
-      </c>
-      <c r="O125" s="1">
-        <f t="shared" si="46"/>
-        <v>4000</v>
-      </c>
-      <c r="P125" s="1">
-        <f t="shared" si="47"/>
         <v>480</v>
       </c>
       <c r="Q125">
@@ -12812,7 +12785,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="126" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>160</v>
       </c>
@@ -12829,11 +12802,11 @@
         <v>120</v>
       </c>
       <c r="F126" s="1" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="46"/>
         <v>Unknown</v>
       </c>
       <c r="G126" s="2" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="47"/>
         <v>Unknown</v>
       </c>
       <c r="H126" t="s">
@@ -12856,15 +12829,15 @@
         <v>16</v>
       </c>
       <c r="N126" s="1">
+        <f t="shared" si="43"/>
+        <v>65536</v>
+      </c>
+      <c r="O126" s="1">
+        <f t="shared" si="44"/>
+        <v>8000</v>
+      </c>
+      <c r="P126" s="1">
         <f t="shared" si="45"/>
-        <v>65536</v>
-      </c>
-      <c r="O126" s="1">
-        <f t="shared" si="46"/>
-        <v>8000</v>
-      </c>
-      <c r="P126" s="1">
-        <f t="shared" si="47"/>
         <v>960</v>
       </c>
       <c r="Q126">
@@ -12901,7 +12874,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="127" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>161</v>
       </c>
@@ -12918,11 +12891,11 @@
         <v>120</v>
       </c>
       <c r="F127" s="1" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="46"/>
         <v>Unknown</v>
       </c>
       <c r="G127" s="2" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="47"/>
         <v>Unknown</v>
       </c>
       <c r="H127" t="s">
@@ -12945,15 +12918,15 @@
         <v>32</v>
       </c>
       <c r="N127" s="1">
+        <f t="shared" si="43"/>
+        <v>131072</v>
+      </c>
+      <c r="O127" s="1">
+        <f t="shared" si="44"/>
+        <v>16000</v>
+      </c>
+      <c r="P127" s="1">
         <f t="shared" si="45"/>
-        <v>131072</v>
-      </c>
-      <c r="O127" s="1">
-        <f t="shared" si="46"/>
-        <v>16000</v>
-      </c>
-      <c r="P127" s="1">
-        <f t="shared" si="47"/>
         <v>1920</v>
       </c>
       <c r="Q127">
@@ -12990,7 +12963,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="128" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>175</v>
       </c>
@@ -13007,11 +12980,11 @@
         <v>120</v>
       </c>
       <c r="F128" s="1" t="str">
-        <f t="shared" ref="F128:F129" si="52">IFERROR(E128*I128,"Unknown")</f>
+        <f t="shared" ref="F128:F129" si="50">IFERROR(E128*I128,"Unknown")</f>
         <v>Unknown</v>
       </c>
       <c r="G128" s="2" t="str">
-        <f t="shared" ref="G128:G129" si="53">IFERROR(C128/F128*1000,"Unknown")</f>
+        <f t="shared" ref="G128:G129" si="51">IFERROR(C128/F128*1000,"Unknown")</f>
         <v>Unknown</v>
       </c>
       <c r="H128" t="s">
@@ -13076,7 +13049,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="129" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>176</v>
       </c>
@@ -13093,11 +13066,11 @@
         <v>120</v>
       </c>
       <c r="F129" s="1" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="50"/>
         <v>Unknown</v>
       </c>
       <c r="G129" s="2" t="str">
-        <f t="shared" si="53"/>
+        <f t="shared" si="51"/>
         <v>Unknown</v>
       </c>
       <c r="H129" t="s">
@@ -13162,7 +13135,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="130" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>162</v>
       </c>
@@ -13179,11 +13152,11 @@
         <v>120</v>
       </c>
       <c r="F130" s="1" t="str">
-        <f t="shared" ref="F130:F135" si="54">IFERROR(E130*I130,"Unknown")</f>
+        <f t="shared" ref="F130:F135" si="52">IFERROR(E130*I130,"Unknown")</f>
         <v>Unknown</v>
       </c>
       <c r="G130" s="2" t="str">
-        <f t="shared" ref="G130:G135" si="55">IFERROR(C130/F130*1000,"Unknown")</f>
+        <f t="shared" ref="G130:G135" si="53">IFERROR(C130/F130*1000,"Unknown")</f>
         <v>Unknown</v>
       </c>
       <c r="H130" t="s">
@@ -13251,7 +13224,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="131" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>163</v>
       </c>
@@ -13268,11 +13241,11 @@
         <v>120</v>
       </c>
       <c r="F131" s="1" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="52"/>
         <v>Unknown</v>
       </c>
       <c r="G131" s="2" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="53"/>
         <v>Unknown</v>
       </c>
       <c r="H131" t="s">
@@ -13295,15 +13268,15 @@
         <v>8</v>
       </c>
       <c r="N131" s="1">
-        <f t="shared" ref="N131:N135" si="56">M131*4*1024</f>
+        <f t="shared" ref="N131:N135" si="54">M131*4*1024</f>
         <v>32768</v>
       </c>
       <c r="O131" s="1">
-        <f t="shared" ref="O131:O135" si="57">M131*500</f>
+        <f t="shared" ref="O131:O135" si="55">M131*500</f>
         <v>4000</v>
       </c>
       <c r="P131" s="1">
-        <f t="shared" ref="P131:P135" si="58">M131*60</f>
+        <f t="shared" ref="P131:P135" si="56">M131*60</f>
         <v>480</v>
       </c>
       <c r="Q131" s="1">
@@ -13340,7 +13313,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="132" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>164</v>
       </c>
@@ -13357,11 +13330,11 @@
         <v>120</v>
       </c>
       <c r="F132" s="1" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="52"/>
         <v>Unknown</v>
       </c>
       <c r="G132" s="2" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="53"/>
         <v>Unknown</v>
       </c>
       <c r="H132" t="s">
@@ -13384,15 +13357,15 @@
         <v>16</v>
       </c>
       <c r="N132" s="1">
+        <f t="shared" si="54"/>
+        <v>65536</v>
+      </c>
+      <c r="O132" s="1">
+        <f t="shared" si="55"/>
+        <v>8000</v>
+      </c>
+      <c r="P132" s="1">
         <f t="shared" si="56"/>
-        <v>65536</v>
-      </c>
-      <c r="O132" s="1">
-        <f t="shared" si="57"/>
-        <v>8000</v>
-      </c>
-      <c r="P132" s="1">
-        <f t="shared" si="58"/>
         <v>960</v>
       </c>
       <c r="Q132" s="1">
@@ -13429,7 +13402,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="133" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>165</v>
       </c>
@@ -13446,11 +13419,11 @@
         <v>120</v>
       </c>
       <c r="F133" s="1" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="52"/>
         <v>Unknown</v>
       </c>
       <c r="G133" s="2" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="53"/>
         <v>Unknown</v>
       </c>
       <c r="H133" t="s">
@@ -13473,15 +13446,15 @@
         <v>32</v>
       </c>
       <c r="N133" s="1">
+        <f t="shared" si="54"/>
+        <v>131072</v>
+      </c>
+      <c r="O133" s="1">
+        <f t="shared" si="55"/>
+        <v>16000</v>
+      </c>
+      <c r="P133" s="1">
         <f t="shared" si="56"/>
-        <v>131072</v>
-      </c>
-      <c r="O133" s="1">
-        <f t="shared" si="57"/>
-        <v>16000</v>
-      </c>
-      <c r="P133" s="1">
-        <f t="shared" si="58"/>
         <v>1920</v>
       </c>
       <c r="Q133" s="1">
@@ -13518,7 +13491,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="134" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>166</v>
       </c>
@@ -13535,11 +13508,11 @@
         <v>120</v>
       </c>
       <c r="F134" s="1" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="52"/>
         <v>Unknown</v>
       </c>
       <c r="G134" s="2" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="53"/>
         <v>Unknown</v>
       </c>
       <c r="H134" t="s">
@@ -13562,15 +13535,15 @@
         <v>64</v>
       </c>
       <c r="N134" s="1">
+        <f t="shared" si="54"/>
+        <v>262144</v>
+      </c>
+      <c r="O134" s="1">
+        <f t="shared" si="55"/>
+        <v>32000</v>
+      </c>
+      <c r="P134" s="1">
         <f t="shared" si="56"/>
-        <v>262144</v>
-      </c>
-      <c r="O134" s="1">
-        <f t="shared" si="57"/>
-        <v>32000</v>
-      </c>
-      <c r="P134" s="1">
-        <f t="shared" si="58"/>
         <v>3840</v>
       </c>
       <c r="Q134" s="1">
@@ -13607,7 +13580,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="135" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>167</v>
       </c>
@@ -13624,11 +13597,11 @@
         <v>120</v>
       </c>
       <c r="F135" s="1" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="52"/>
         <v>Unknown</v>
       </c>
       <c r="G135" s="2" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="53"/>
         <v>Unknown</v>
       </c>
       <c r="H135" t="s">
@@ -13651,15 +13624,15 @@
         <v>64</v>
       </c>
       <c r="N135" s="1">
+        <f t="shared" si="54"/>
+        <v>262144</v>
+      </c>
+      <c r="O135" s="1">
+        <f t="shared" si="55"/>
+        <v>32000</v>
+      </c>
+      <c r="P135" s="1">
         <f t="shared" si="56"/>
-        <v>262144</v>
-      </c>
-      <c r="O135" s="1">
-        <f t="shared" si="57"/>
-        <v>32000</v>
-      </c>
-      <c r="P135" s="1">
-        <f t="shared" si="58"/>
         <v>3840</v>
       </c>
       <c r="Q135" s="1">

</xml_diff>

<commit_message>
Fixed GS5 in regards to HANA support
</commit_message>
<xml_diff>
--- a/AzureVMSizes.xlsx
+++ b/AzureVMSizes.xlsx
@@ -1410,11 +1410,11 @@
   <dimension ref="A1:AA135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2676" ySplit="576" topLeftCell="Q124" activePane="bottomRight"/>
+      <pane xSplit="2676" ySplit="576" topLeftCell="Q73" activePane="bottomRight"/>
       <selection sqref="A1:A1048576"/>
       <selection pane="topRight" activeCell="AA1" sqref="AA1"/>
       <selection pane="bottomLeft" activeCell="A129" sqref="A129"/>
-      <selection pane="bottomRight" activeCell="Z16" sqref="Z16"/>
+      <selection pane="bottomRight" activeCell="Z92" sqref="Z92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9709,7 +9709,7 @@
         <v>144</v>
       </c>
       <c r="Z91" s="1" t="s">
-        <v>143</v>
+        <v>177</v>
       </c>
       <c r="AA91" t="s">
         <v>108</v>
@@ -10685,7 +10685,7 @@
         <v>4000</v>
       </c>
       <c r="U102" s="2">
-        <f t="shared" ref="U102:W111" si="37">IFERROR(Q102/T102*1000,"Unknown")</f>
+        <f t="shared" ref="U102:V111" si="37">IFERROR(Q102/T102*1000,"Unknown")</f>
         <v>20000</v>
       </c>
       <c r="V102" s="2">

</xml_diff>

<commit_message>
Updated missing pricing in regards to low priority pricing for Ev3/Dv3/N and NC pricing
</commit_message>
<xml_diff>
--- a/AzureVMSizes.xlsx
+++ b/AzureVMSizes.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1358" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1327" uniqueCount="178">
   <si>
     <t>Name</t>
   </si>
@@ -1410,11 +1410,11 @@
   <dimension ref="A1:AA135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2676" ySplit="576" topLeftCell="Q73" activePane="bottomRight"/>
+      <pane xSplit="2676" ySplit="576" topLeftCell="A103" activePane="bottomRight"/>
       <selection sqref="A1:A1048576"/>
       <selection pane="topRight" activeCell="AA1" sqref="AA1"/>
       <selection pane="bottomLeft" activeCell="A129" sqref="A129"/>
-      <selection pane="bottomRight" activeCell="Z92" sqref="Z92"/>
+      <selection pane="bottomRight" activeCell="D130" sqref="D130:D135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10897,11 +10897,11 @@
       <c r="B105" t="s">
         <v>129</v>
       </c>
-      <c r="C105" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>120</v>
+      <c r="C105" s="1">
+        <v>1.968</v>
+      </c>
+      <c r="D105" s="1">
+        <v>0.36899999999999999</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>120</v>
@@ -10990,11 +10990,11 @@
       <c r="B106" t="s">
         <v>129</v>
       </c>
-      <c r="C106" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>120</v>
+      <c r="C106" s="1">
+        <v>3.9350000000000001</v>
+      </c>
+      <c r="D106" s="1">
+        <v>0.73799999999999999</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>120</v>
@@ -11083,8 +11083,8 @@
       <c r="B107" t="s">
         <v>129</v>
       </c>
-      <c r="C107" s="1" t="s">
-        <v>120</v>
+      <c r="C107" s="1">
+        <v>4.3280000000000003</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>120</v>
@@ -11176,11 +11176,11 @@
       <c r="B108" t="s">
         <v>129</v>
       </c>
-      <c r="C108" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>120</v>
+      <c r="C108" s="1">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="D108" s="1">
+        <v>0.185</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>120</v>
@@ -11551,8 +11551,8 @@
       <c r="C112" s="1">
         <v>0.13500000000000001</v>
       </c>
-      <c r="D112" s="1" t="s">
-        <v>123</v>
+      <c r="D112" s="1">
+        <v>2.3E-2</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>120</v>
@@ -11640,8 +11640,8 @@
       <c r="C113" s="1">
         <v>0.27</v>
       </c>
-      <c r="D113" s="1" t="s">
-        <v>123</v>
+      <c r="D113" s="1">
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>120</v>
@@ -11729,8 +11729,8 @@
       <c r="C114" s="1">
         <v>0.54</v>
       </c>
-      <c r="D114" s="1" t="s">
-        <v>123</v>
+      <c r="D114" s="1">
+        <v>0.09</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>120</v>
@@ -11818,8 +11818,8 @@
       <c r="C115" s="1">
         <v>1.08</v>
       </c>
-      <c r="D115" s="1" t="s">
-        <v>123</v>
+      <c r="D115" s="1">
+        <v>0.18</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>120</v>
@@ -11907,8 +11907,8 @@
       <c r="C116" s="1">
         <v>2.1589999999999998</v>
       </c>
-      <c r="D116" s="1" t="s">
-        <v>123</v>
+      <c r="D116" s="1">
+        <v>0.36</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>120</v>
@@ -11996,8 +11996,8 @@
       <c r="C117" s="1">
         <v>4.07</v>
       </c>
-      <c r="D117" s="1" t="s">
-        <v>123</v>
+      <c r="D117" s="1">
+        <v>0.67700000000000005</v>
       </c>
       <c r="E117" s="1" t="s">
         <v>120</v>
@@ -12085,8 +12085,8 @@
       <c r="C118" s="1">
         <v>0.10199999999999999</v>
       </c>
-      <c r="D118" s="1" t="s">
-        <v>123</v>
+      <c r="D118" s="1">
+        <v>1.9E-2</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>120</v>
@@ -12175,8 +12175,8 @@
       <c r="C119" s="1">
         <v>0.20300000000000001</v>
       </c>
-      <c r="D119" s="1" t="s">
-        <v>123</v>
+      <c r="D119" s="1">
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>120</v>
@@ -12265,8 +12265,8 @@
       <c r="C120" s="1">
         <v>0.40500000000000003</v>
       </c>
-      <c r="D120" s="1" t="s">
-        <v>123</v>
+      <c r="D120" s="1">
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>120</v>
@@ -12355,8 +12355,8 @@
       <c r="C121" s="1">
         <v>0.81</v>
       </c>
-      <c r="D121" s="1" t="s">
-        <v>123</v>
+      <c r="D121" s="1">
+        <v>0.14599999999999999</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>120</v>
@@ -12445,8 +12445,8 @@
       <c r="C122" s="1">
         <v>1.62</v>
       </c>
-      <c r="D122" s="1" t="s">
-        <v>123</v>
+      <c r="D122" s="1">
+        <v>0.29099999999999998</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>120</v>
@@ -12531,8 +12531,8 @@
       <c r="C123" s="1">
         <v>3.2389999999999999</v>
       </c>
-      <c r="D123" s="1" t="s">
-        <v>123</v>
+      <c r="D123" s="1">
+        <v>0.58199999999999996</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>120</v>
@@ -12617,8 +12617,8 @@
       <c r="C124" s="1">
         <v>0.10199999999999999</v>
       </c>
-      <c r="D124" s="1" t="s">
-        <v>123</v>
+      <c r="D124" s="1">
+        <v>1.9E-2</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>120</v>
@@ -12706,8 +12706,8 @@
       <c r="C125" s="1">
         <v>0.20300000000000001</v>
       </c>
-      <c r="D125" s="1" t="s">
-        <v>123</v>
+      <c r="D125" s="1">
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>120</v>
@@ -12795,8 +12795,8 @@
       <c r="C126" s="1">
         <v>0.40500000000000003</v>
       </c>
-      <c r="D126" s="1" t="s">
-        <v>123</v>
+      <c r="D126" s="1">
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>120</v>
@@ -12884,8 +12884,8 @@
       <c r="C127" s="1">
         <v>0.81</v>
       </c>
-      <c r="D127" s="1" t="s">
-        <v>123</v>
+      <c r="D127" s="1">
+        <v>0.14599999999999999</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>120</v>
@@ -12973,8 +12973,8 @@
       <c r="C128" s="1">
         <v>1.62</v>
       </c>
-      <c r="D128" s="1" t="s">
-        <v>123</v>
+      <c r="D128" s="1">
+        <v>0.29099999999999998</v>
       </c>
       <c r="E128" s="1" t="s">
         <v>120</v>
@@ -13059,8 +13059,8 @@
       <c r="C129" s="1">
         <v>3.2389999999999999</v>
       </c>
-      <c r="D129" s="1" t="s">
-        <v>123</v>
+      <c r="D129" s="1">
+        <v>0.58199999999999996</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>120</v>
@@ -13145,8 +13145,8 @@
       <c r="C130" s="1">
         <v>0.13500000000000001</v>
       </c>
-      <c r="D130" s="1" t="s">
-        <v>123</v>
+      <c r="D130" s="1">
+        <v>2.3E-2</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>120</v>
@@ -13234,8 +13234,8 @@
       <c r="C131" s="1">
         <v>0.27</v>
       </c>
-      <c r="D131" s="1" t="s">
-        <v>123</v>
+      <c r="D131" s="1">
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="E131" s="1" t="s">
         <v>120</v>
@@ -13323,8 +13323,8 @@
       <c r="C132" s="1">
         <v>0.54</v>
       </c>
-      <c r="D132" s="1" t="s">
-        <v>123</v>
+      <c r="D132" s="1">
+        <v>0.09</v>
       </c>
       <c r="E132" s="1" t="s">
         <v>120</v>
@@ -13412,8 +13412,8 @@
       <c r="C133" s="1">
         <v>1.08</v>
       </c>
-      <c r="D133" s="1" t="s">
-        <v>123</v>
+      <c r="D133" s="1">
+        <v>0.18</v>
       </c>
       <c r="E133" s="1" t="s">
         <v>120</v>
@@ -13501,8 +13501,8 @@
       <c r="C134" s="1">
         <v>2.1589999999999998</v>
       </c>
-      <c r="D134" s="1" t="s">
-        <v>123</v>
+      <c r="D134" s="1">
+        <v>0.36</v>
       </c>
       <c r="E134" s="1" t="s">
         <v>120</v>
@@ -13590,8 +13590,8 @@
       <c r="C135" s="1">
         <v>4.07</v>
       </c>
-      <c r="D135" s="1" t="s">
-        <v>123</v>
+      <c r="D135" s="1">
+        <v>0.67700000000000005</v>
       </c>
       <c r="E135" s="1" t="s">
         <v>120</v>

</xml_diff>

<commit_message>
Updated E-series indicating hyperthreaded
</commit_message>
<xml_diff>
--- a/AzureVMSizes.xlsx
+++ b/AzureVMSizes.xlsx
@@ -1410,11 +1410,11 @@
   <dimension ref="A1:AA135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2676" ySplit="576" topLeftCell="A103" activePane="bottomRight"/>
+      <pane xSplit="2676" ySplit="576" topLeftCell="Q1" activePane="bottomRight"/>
       <selection sqref="A1:A1048576"/>
       <selection pane="topRight" activeCell="AA1" sqref="AA1"/>
       <selection pane="bottomLeft" activeCell="A129" sqref="A129"/>
-      <selection pane="bottomRight" activeCell="D130" sqref="D130:D135"/>
+      <selection pane="bottomRight" activeCell="AA129" sqref="AA129:AA135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11627,7 +11627,7 @@
         <v>143</v>
       </c>
       <c r="AA112" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="113" spans="1:27" x14ac:dyDescent="0.3">
@@ -11716,7 +11716,7 @@
         <v>143</v>
       </c>
       <c r="AA113" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="114" spans="1:27" x14ac:dyDescent="0.3">
@@ -11805,7 +11805,7 @@
         <v>143</v>
       </c>
       <c r="AA114" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="115" spans="1:27" x14ac:dyDescent="0.3">
@@ -11894,7 +11894,7 @@
         <v>143</v>
       </c>
       <c r="AA115" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="116" spans="1:27" x14ac:dyDescent="0.3">
@@ -11983,7 +11983,7 @@
         <v>143</v>
       </c>
       <c r="AA116" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="117" spans="1:27" x14ac:dyDescent="0.3">
@@ -12072,7 +12072,7 @@
         <v>143</v>
       </c>
       <c r="AA117" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="118" spans="1:27" x14ac:dyDescent="0.3">
@@ -13221,7 +13221,7 @@
         <v>143</v>
       </c>
       <c r="AA130" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="131" spans="1:27" x14ac:dyDescent="0.3">
@@ -13310,7 +13310,7 @@
         <v>143</v>
       </c>
       <c r="AA131" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="132" spans="1:27" x14ac:dyDescent="0.3">
@@ -13399,7 +13399,7 @@
         <v>143</v>
       </c>
       <c r="AA132" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="133" spans="1:27" x14ac:dyDescent="0.3">
@@ -13488,7 +13488,7 @@
         <v>143</v>
       </c>
       <c r="AA133" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="134" spans="1:27" x14ac:dyDescent="0.3">
@@ -13577,7 +13577,7 @@
         <v>143</v>
       </c>
       <c r="AA134" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="135" spans="1:27" x14ac:dyDescent="0.3">
@@ -13666,7 +13666,7 @@
         <v>143</v>
       </c>
       <c r="AA135" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added first info from the new B-series
</commit_message>
<xml_diff>
--- a/AzureVMSizes.xlsx
+++ b/AzureVMSizes.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1327" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1447" uniqueCount="184">
   <si>
     <t>Name</t>
   </si>
@@ -556,6 +556,24 @@
   </si>
   <si>
     <t>Supported</t>
+  </si>
+  <si>
+    <t>Standard_B1S</t>
+  </si>
+  <si>
+    <t>Standard_B2S</t>
+  </si>
+  <si>
+    <t>Standard_B1MS</t>
+  </si>
+  <si>
+    <t>Standard_B2MS</t>
+  </si>
+  <si>
+    <t>Standard_B4MS</t>
+  </si>
+  <si>
+    <t>Standard_B8MS</t>
   </si>
 </sst>
 </file>
@@ -1407,14 +1425,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA135"/>
+  <dimension ref="A1:AA141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2676" ySplit="576" topLeftCell="Q1" activePane="bottomRight"/>
+      <pane xSplit="2676" ySplit="576" topLeftCell="A124" activePane="bottomRight"/>
       <selection sqref="A1:A1048576"/>
       <selection pane="topRight" activeCell="AA1" sqref="AA1"/>
-      <selection pane="bottomLeft" activeCell="A129" sqref="A129"/>
-      <selection pane="bottomRight" activeCell="AA129" sqref="AA129:AA135"/>
+      <selection pane="bottomLeft" activeCell="A141" sqref="A141"/>
+      <selection pane="bottomRight" activeCell="C150" sqref="C150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13669,6 +13687,519 @@
         <v>109</v>
       </c>
     </row>
+    <row r="136" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>178</v>
+      </c>
+      <c r="B136" t="s">
+        <v>129</v>
+      </c>
+      <c r="C136" s="1">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F136" s="1" t="str">
+        <f t="shared" ref="F136:F141" si="57">IFERROR(E136*I136,"Unknown")</f>
+        <v>Unknown</v>
+      </c>
+      <c r="G136" s="2" t="str">
+        <f t="shared" ref="G136:G141" si="58">IFERROR(C136/F136*1000,"Unknown")</f>
+        <v>Unknown</v>
+      </c>
+      <c r="H136" t="s">
+        <v>108</v>
+      </c>
+      <c r="I136">
+        <v>1</v>
+      </c>
+      <c r="J136">
+        <v>1024</v>
+      </c>
+      <c r="K136" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L136" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="M136" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="N136" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="O136" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="P136" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q136" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="R136" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="S136">
+        <v>2000</v>
+      </c>
+      <c r="T136" s="1">
+        <v>2</v>
+      </c>
+      <c r="U136" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="V136" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="W136" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="X136" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y136" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z136" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA136" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="137" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>179</v>
+      </c>
+      <c r="B137" t="s">
+        <v>129</v>
+      </c>
+      <c r="C137" s="1">
+        <v>2.3E-2</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F137" s="1" t="str">
+        <f t="shared" si="57"/>
+        <v>Unknown</v>
+      </c>
+      <c r="G137" s="2" t="str">
+        <f t="shared" si="58"/>
+        <v>Unknown</v>
+      </c>
+      <c r="H137" t="s">
+        <v>108</v>
+      </c>
+      <c r="I137">
+        <v>2</v>
+      </c>
+      <c r="J137">
+        <v>4096</v>
+      </c>
+      <c r="K137" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L137" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="M137" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="N137" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="O137" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="P137" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q137" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="R137" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="S137">
+        <v>8000</v>
+      </c>
+      <c r="T137" s="1">
+        <v>8</v>
+      </c>
+      <c r="U137" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="V137" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="W137" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="X137" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y137" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z137" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA137" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="138" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>180</v>
+      </c>
+      <c r="B138" t="s">
+        <v>129</v>
+      </c>
+      <c r="C138" s="1">
+        <v>1.2E-2</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F138" s="1" t="str">
+        <f t="shared" si="57"/>
+        <v>Unknown</v>
+      </c>
+      <c r="G138" s="2" t="str">
+        <f t="shared" si="58"/>
+        <v>Unknown</v>
+      </c>
+      <c r="H138" t="s">
+        <v>108</v>
+      </c>
+      <c r="I138">
+        <v>1</v>
+      </c>
+      <c r="J138">
+        <v>2048</v>
+      </c>
+      <c r="K138" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L138" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="M138" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="N138" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="O138" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="P138" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q138" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="R138" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="S138">
+        <v>4000</v>
+      </c>
+      <c r="T138" s="1">
+        <v>4</v>
+      </c>
+      <c r="U138" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="V138" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="W138" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="X138" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y138" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z138" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA138" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="139" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>181</v>
+      </c>
+      <c r="B139" t="s">
+        <v>129</v>
+      </c>
+      <c r="C139" s="1">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E139" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F139" s="1" t="str">
+        <f t="shared" si="57"/>
+        <v>Unknown</v>
+      </c>
+      <c r="G139" s="2" t="str">
+        <f t="shared" si="58"/>
+        <v>Unknown</v>
+      </c>
+      <c r="H139" t="s">
+        <v>108</v>
+      </c>
+      <c r="I139">
+        <v>2</v>
+      </c>
+      <c r="J139">
+        <f>8*1024</f>
+        <v>8192</v>
+      </c>
+      <c r="K139" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L139" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="M139" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="N139" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="O139" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="P139" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q139" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="R139" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="S139">
+        <v>16000</v>
+      </c>
+      <c r="T139" s="1">
+        <v>16</v>
+      </c>
+      <c r="U139" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="V139" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="W139" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="X139" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y139" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z139" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA139" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="140" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>182</v>
+      </c>
+      <c r="B140" t="s">
+        <v>129</v>
+      </c>
+      <c r="C140" s="1">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E140" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F140" s="1" t="str">
+        <f t="shared" si="57"/>
+        <v>Unknown</v>
+      </c>
+      <c r="G140" s="2" t="str">
+        <f t="shared" si="58"/>
+        <v>Unknown</v>
+      </c>
+      <c r="H140" t="s">
+        <v>108</v>
+      </c>
+      <c r="I140">
+        <v>4</v>
+      </c>
+      <c r="J140">
+        <f>16*1024</f>
+        <v>16384</v>
+      </c>
+      <c r="K140" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L140" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="M140" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="N140" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="O140" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="P140" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q140" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="R140" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="S140">
+        <v>32000</v>
+      </c>
+      <c r="T140" s="1">
+        <v>32</v>
+      </c>
+      <c r="U140" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="V140" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="W140" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="X140" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y140" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z140" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA140" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="141" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>183</v>
+      </c>
+      <c r="B141" t="s">
+        <v>129</v>
+      </c>
+      <c r="C141" s="1">
+        <v>0.183</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E141" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F141" s="1" t="str">
+        <f t="shared" si="57"/>
+        <v>Unknown</v>
+      </c>
+      <c r="G141" s="2" t="str">
+        <f t="shared" si="58"/>
+        <v>Unknown</v>
+      </c>
+      <c r="H141" t="s">
+        <v>108</v>
+      </c>
+      <c r="I141">
+        <v>8</v>
+      </c>
+      <c r="J141">
+        <f>32*1024</f>
+        <v>32768</v>
+      </c>
+      <c r="K141" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L141" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="M141" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="N141" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="O141" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="P141" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q141" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="R141" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="S141">
+        <v>64000</v>
+      </c>
+      <c r="T141" s="1">
+        <v>64</v>
+      </c>
+      <c r="U141" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="V141" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="W141" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="X141" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y141" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z141" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA141" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:T2169">
     <sortState ref="A2:T111">

</xml_diff>